<commit_message>
Testberechnungen / Nutzenergiebedarf fertig
</commit_message>
<xml_diff>
--- a/din18599/Testberechnungen.xlsx
+++ b/din18599/Testberechnungen.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wagesve/Awesome/_Kunden/Energieausweis online erstellen/Dokumente/DIN V 18599/Wohngebäude/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wagesve/Dev/Sites/enon/din18599/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2731F8A-2F9D-CC4D-8CA2-10774895416D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AFE753-7760-1247-BB78-51C6280C1A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{7CF02650-DC02-AA49-AC3A-4487EF2FF614}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{7CF02650-DC02-AA49-AC3A-4487EF2FF614}"/>
   </bookViews>
   <sheets>
     <sheet name="Gebäude" sheetId="1" r:id="rId1"/>
     <sheet name="Dach" sheetId="2" r:id="rId2"/>
-    <sheet name="Wärmequellen" sheetId="3" r:id="rId3"/>
-    <sheet name="Tabelle1" sheetId="4" r:id="rId4"/>
+    <sheet name="Bilanzierung" sheetId="3" r:id="rId3"/>
+    <sheet name="Heizsystem" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="181">
   <si>
     <t>Haus Rechteckig</t>
   </si>
@@ -525,9 +525,6 @@
     <t>Qi</t>
   </si>
   <si>
-    <t>Korrekturfakoren und weitere Werte</t>
-  </si>
-  <si>
     <t>pi</t>
   </si>
   <si>
@@ -547,13 +544,73 @@
   </si>
   <si>
     <t>thm</t>
+  </si>
+  <si>
+    <t>ßhma</t>
+  </si>
+  <si>
+    <t>thm 1</t>
+  </si>
+  <si>
+    <t>thm 2</t>
+  </si>
+  <si>
+    <t>Nutzenergiebedarf</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>qh</t>
+  </si>
+  <si>
+    <t>flna</t>
+  </si>
+  <si>
+    <t>1 - ( ( 10 - $this-&gt;monatsdaten-&gt;temperatur( $monat ) ) / 22 );</t>
+  </si>
+  <si>
+    <t>flna temp</t>
+  </si>
+  <si>
+    <t>Temperaturen</t>
+  </si>
+  <si>
+    <t>ehd</t>
+  </si>
+  <si>
+    <t>ehd0 Einfamilienhäuser</t>
+  </si>
+  <si>
+    <t>Vorlauftemperatur Übergabe</t>
+  </si>
+  <si>
+    <t>Standort Heizung</t>
+  </si>
+  <si>
+    <t>ausserhalb</t>
+  </si>
+  <si>
+    <t>90/70</t>
+  </si>
+  <si>
+    <t>70/55</t>
+  </si>
+  <si>
+    <t>55/45</t>
+  </si>
+  <si>
+    <t>35/28</t>
+  </si>
+  <si>
+    <t>Berechnung Satteldach</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -581,12 +638,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -629,7 +680,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -700,68 +751,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -774,35 +763,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1117,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D0A30B-5A9B-F949-B5FE-8B73CA8912C0}">
-  <dimension ref="A1:P78"/>
+  <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView topLeftCell="D23" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1135,9 +1122,11 @@
     <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.5" customWidth="1"/>
+    <col min="18" max="18" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1148,7 +1137,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1174,8 +1163,11 @@
       <c r="P3" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R3" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1200,14 +1192,14 @@
         <v>1</v>
       </c>
       <c r="K4">
-        <f>Dach!E3</f>
+        <f>Gebäude!S5</f>
         <v>10</v>
       </c>
       <c r="M4" t="s">
         <v>1</v>
       </c>
       <c r="N4">
-        <f>Dach!$E$6</f>
+        <f>Gebäude!$S$8</f>
         <v>7.5</v>
       </c>
       <c r="P4">
@@ -1215,7 +1207,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1233,7 +1225,7 @@
         <v>2</v>
       </c>
       <c r="K5">
-        <f>Dach!E4</f>
+        <f>Gebäude!S6</f>
         <v>15</v>
       </c>
       <c r="M5" t="s">
@@ -1246,8 +1238,15 @@
         <f t="shared" ref="P5:P7" si="0">H5+K5+N5</f>
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R5" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5">
+        <f>Dach!B3*Dach!B5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1265,22 +1264,29 @@
         <v>28</v>
       </c>
       <c r="K6">
-        <f>Dach!E3</f>
+        <f>Gebäude!S5</f>
         <v>10</v>
       </c>
       <c r="M6" t="s">
         <v>28</v>
       </c>
       <c r="N6">
-        <f>Dach!$E$6</f>
+        <f>Gebäude!$S$8</f>
         <v>7.5</v>
       </c>
       <c r="P6">
         <f t="shared" si="0"/>
         <v>67.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R6" t="s">
+        <v>17</v>
+      </c>
+      <c r="S6">
+        <f>Dach!B3*Dach!B6</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -1302,7 +1308,7 @@
         <v>29</v>
       </c>
       <c r="K7" s="4">
-        <f>Dach!E4</f>
+        <f>Gebäude!S6</f>
         <v>15</v>
       </c>
       <c r="L7" s="4"/>
@@ -1317,8 +1323,15 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R7" t="s">
+        <v>18</v>
+      </c>
+      <c r="S7">
+        <f xml:space="preserve"> S5*2+S6*2</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1344,8 +1357,15 @@
         <f t="shared" si="1"/>
         <v>315</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R8" t="s">
+        <v>19</v>
+      </c>
+      <c r="S8">
+        <f>(Dach!B4-Dach!B3)*(Dach!B5/2)</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1353,8 +1373,15 @@
         <v>0.25</v>
       </c>
       <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R9" t="s">
+        <v>35</v>
+      </c>
+      <c r="S9">
+        <f>SQRT(SUMSQ(Dach!B7)+SUMSQ(Dach!B5/2))</f>
+        <v>5.2201532544552753</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1384,7 +1411,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -1421,8 +1448,15 @@
         <f t="array" ref="M11">_xlfn.SWITCH(B7,"Nord", I11,"Ost",I12,"Süd",I13,"West",I14)</f>
         <v>7.8375000000000004</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R11" t="s">
+        <v>15</v>
+      </c>
+      <c r="S11">
+        <f>Dach!B5*Dach!B6*Dach!B3</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -1459,8 +1493,15 @@
         <f t="array" ref="M12">_xlfn.SWITCH(B7,"Nord",I12,"Ost",I11,"Süd",I14,"West",I13)</f>
         <v>11.9625</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S12">
+        <f>S8*Dach!B6</f>
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1491,7 +1532,7 @@
         <v>7.8375000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1521,8 +1562,11 @@
         <f t="array" ref="M14">_xlfn.SWITCH($B$7,"Nord",I14,"Ost",I13,"Süd",I12,"West",I11)</f>
         <v>11.9625</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R14" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -1530,8 +1574,15 @@
         <f>B12*B14</f>
         <v>769.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R15" t="s">
+        <v>2</v>
+      </c>
+      <c r="S15">
+        <f>S9*Dach!B6</f>
+        <v>78.302298816829136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -1543,8 +1594,15 @@
         <v>27</v>
       </c>
       <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="R16" t="s">
+        <v>29</v>
+      </c>
+      <c r="S16">
+        <f>S9*Dach!B6</f>
+        <v>78.302298816829136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>92</v>
       </c>
@@ -1566,8 +1624,15 @@
         <f>I17*$B$28*$C$28</f>
         <v>4.7024999999999997</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="R17" t="s">
+        <v>11</v>
+      </c>
+      <c r="S17">
+        <f>S15+S16</f>
+        <v>156.60459763365827</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -1591,7 +1656,7 @@
         <v>7.1775000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>105</v>
       </c>
@@ -1614,7 +1679,7 @@
         <v>4.7024999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="G20" t="s">
         <v>29</v>
       </c>
@@ -1631,7 +1696,7 @@
         <v>7.1775000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1639,7 +1704,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1651,7 +1716,7 @@
       </c>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="G23" t="s">
         <v>1</v>
       </c>
@@ -1668,7 +1733,7 @@
         <v>0.70537500000000009</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
@@ -1691,7 +1756,7 @@
         <v>1.0766250000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -1717,7 +1782,7 @@
         <v>0.70537500000000009</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -1743,7 +1808,7 @@
         <v>1.0766250000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -1754,7 +1819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1770,7 +1835,7 @@
       </c>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1792,7 +1857,7 @@
         <v>32.975999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -1814,7 +1879,7 @@
         <v>42.515999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="G31" t="s">
         <v>28</v>
       </c>
@@ -1827,7 +1892,7 @@
         <v>32.975999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>109</v>
       </c>
@@ -1891,7 +1956,7 @@
         <v>37</v>
       </c>
       <c r="H36">
-        <f>Dach!E15</f>
+        <f>Gebäude!S17</f>
         <v>156.60459763365827</v>
       </c>
       <c r="J36">
@@ -1930,16 +1995,16 @@
       <c r="A40" t="s">
         <v>83</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="7">
         <v>0.47099999999999997</v>
       </c>
-      <c r="C40" s="6"/>
+      <c r="C40" s="5"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>84</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="7">
         <v>1.0660000000000001</v>
       </c>
       <c r="G41" s="2" t="s">
@@ -1950,7 +2015,7 @@
       <c r="A42" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="7">
         <v>0.79</v>
       </c>
       <c r="G42" t="s">
@@ -2024,7 +2089,7 @@
       <c r="B48" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="7"/>
+      <c r="C48" s="6"/>
       <c r="G48" s="2" t="s">
         <v>148</v>
       </c>
@@ -2081,7 +2146,7 @@
       <c r="A52" t="s">
         <v>99</v>
       </c>
-      <c r="B52" s="8">
+      <c r="B52" s="7">
         <v>0.79</v>
       </c>
       <c r="G52" s="1" t="s">
@@ -2176,7 +2241,7 @@
         <f>(B37+B43-0.5*B15*0.34*(B52-B51))*32</f>
         <v>15427.801052661227</v>
       </c>
-      <c r="C58" s="7"/>
+      <c r="C58" s="6"/>
       <c r="G58" s="1" t="s">
         <v>63</v>
       </c>
@@ -2196,7 +2261,7 @@
         <f>(B43-0.5*B15*0.34*(B52-B51))*32</f>
         <v>3512.606202950401</v>
       </c>
-      <c r="C59" s="7"/>
+      <c r="C59" s="6"/>
       <c r="G59" s="1" t="s">
         <v>64</v>
       </c>
@@ -2216,7 +2281,7 @@
         <f>IF(B49="Ja",B58,B59)</f>
         <v>3512.606202950401</v>
       </c>
-      <c r="C60" s="7"/>
+      <c r="C60" s="6"/>
       <c r="G60" s="1" t="s">
         <v>65</v>
       </c>
@@ -2271,81 +2336,11 @@
       <c r="A69" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B69" s="8">
+      <c r="B69" s="7">
         <v>8.5</v>
       </c>
       <c r="C69" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>141</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C72" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>145</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>137</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C74" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>146</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>143</v>
-      </c>
-      <c r="B76">
-        <f>IF(B74="innerhalb",IF(B75="Ja",1.554,0.647),IF(B75="Ja",0.815,0.335))</f>
-        <v>1.554</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>144</v>
-      </c>
-      <c r="B77">
-        <f>IF(B75="Ja",1.321,0.451)</f>
-        <v>1.321</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B78" s="2">
-        <f>IF(B72="Ja",IF(B73="Ja",B76,B77),0.193)</f>
-        <v>1.321</v>
       </c>
     </row>
   </sheetData>
@@ -2356,10 +2351,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CF28B4-6980-5D4B-8184-D8E1A3E7B562}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="D2" sqref="D2:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2369,72 +2364,44 @@
     <col min="5" max="5" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3">
-        <f>B3*B5</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>2.5</v>
       </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4">
-        <f>B3*B6</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5">
-        <f xml:space="preserve"> E3*2+E4*2</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>39</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6">
-        <f>(B4-B3)*(B5/2)</f>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -2442,70 +2409,13 @@
         <f>B4-B3</f>
         <v>1.5</v>
       </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7">
-        <f>SQRT(SUMSQ(B7)+SUMSQ(B5/2))</f>
-        <v>5.2201532544552753</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9">
-        <f>B5*B6*B3</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10">
-        <f>E6*B6</f>
-        <v>112.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D12" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <f>E7*B6</f>
-        <v>78.302298816829136</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14">
-        <f>E7*B6</f>
-        <v>78.302298816829136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15">
-        <f>E13+E14</f>
-        <v>156.60459763365827</v>
-      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20">
-        <f>E10+E9</f>
+        <f>Gebäude!S12+Gebäude!S11</f>
         <v>262.5</v>
       </c>
     </row>
@@ -2517,10 +2427,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A340B5-F068-DF4D-BA05-F7AD24B208A4}">
-  <dimension ref="B2:AF40"/>
+  <dimension ref="B2:AF41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView topLeftCell="A2" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2530,14 +2440,15 @@
     <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" customWidth="1"/>
     <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.33203125" customWidth="1"/>
     <col min="16" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" customWidth="1"/>
+    <col min="20" max="20" width="14.5" customWidth="1"/>
     <col min="22" max="22" width="35.33203125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -2554,7 +2465,7 @@
       <c r="E2" t="s">
         <v>150</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="G2" t="s">
@@ -2576,16 +2487,16 @@
         <f>Gebäude!B34</f>
         <v>0.78</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="10"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="9"/>
     </row>
     <row r="4" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
@@ -2605,8 +2516,8 @@
         <f>0.9*1*0.9*0.7*I3</f>
         <v>0.44225999999999999</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="15" t="s">
+      <c r="J4" s="6"/>
+      <c r="K4" s="14" t="s">
         <v>118</v>
       </c>
       <c r="L4" s="4">
@@ -2630,7 +2541,7 @@
       <c r="Q4" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="R4" s="16">
+      <c r="R4" s="15">
         <f>Gebäude!M14</f>
         <v>11.9625</v>
       </c>
@@ -2645,31 +2556,31 @@
         <v>147</v>
       </c>
       <c r="Y4">
-        <f>Gebäude!B78</f>
+        <f>Heizsystem!C9</f>
         <v>1.321</v>
       </c>
     </row>
-    <row r="5" spans="2:32" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="I6" s="9"/>
+      <c r="J6" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="17" t="s">
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="9"/>
       <c r="T6" s="2" t="s">
         <v>133</v>
       </c>
@@ -2680,7 +2591,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="2:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>54</v>
       </c>
@@ -2696,37 +2607,37 @@
       <c r="F7" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="L7" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="M7" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="O7" s="21" t="s">
+      <c r="O7" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="P7" s="21" t="s">
+      <c r="P7" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="Q7" s="21" t="s">
+      <c r="Q7" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="R7" s="22" t="s">
+      <c r="R7" s="18" t="s">
         <v>128</v>
       </c>
       <c r="T7" s="2" t="s">
@@ -2826,7 +2737,7 @@
         <v>31</v>
       </c>
       <c r="AC8">
-        <f>H23*(D23/$D$36)*$F$2/Gebäude!I50</f>
+        <f>H24*(D24/$D$37)*$F$2/Gebäude!I50</f>
         <v>407.92431028289218</v>
       </c>
       <c r="AE8" t="s">
@@ -2871,7 +2782,7 @@
       <c r="L9">
         <v>47</v>
       </c>
-      <c r="M9" s="14">
+      <c r="M9" s="13">
         <v>24</v>
       </c>
       <c r="N9">
@@ -2915,7 +2826,7 @@
         <v>28</v>
       </c>
       <c r="AC9">
-        <f>H24*(D24/$D$36)*$F$2/Gebäude!I51</f>
+        <f>H25*(D25/$D$37)*$F$2/Gebäude!I51</f>
         <v>335.4194047700654</v>
       </c>
       <c r="AE9" t="s">
@@ -3004,7 +2915,7 @@
         <v>31</v>
       </c>
       <c r="AC10">
-        <f>H25*(D25/$D$36)*$F$2/Gebäude!I52</f>
+        <f>H26*(D26/$D$37)*$F$2/Gebäude!I52</f>
         <v>74.728302090693319</v>
       </c>
       <c r="AE10" t="s">
@@ -3093,7 +3004,7 @@
         <v>30</v>
       </c>
       <c r="AC11">
-        <f>H26*(D26/$D$36)*$F$2/Gebäude!I53</f>
+        <f>H27*(D27/$D$37)*$F$2/Gebäude!I53</f>
         <v>104.9733351337067</v>
       </c>
       <c r="AE11" t="s">
@@ -3182,7 +3093,7 @@
         <v>31</v>
       </c>
       <c r="AC12">
-        <f>H27*(D27/$D$36)*$F$2/Gebäude!I54</f>
+        <f>H28*(D28/$D$37)*$F$2/Gebäude!I54</f>
         <v>23.095391516545366</v>
       </c>
       <c r="AE12" t="s">
@@ -3271,7 +3182,7 @@
         <v>30</v>
       </c>
       <c r="AC13">
-        <f>H28*(D28/$D$36)*$F$2/Gebäude!I55</f>
+        <f>H29*(D29/$D$37)*$F$2/Gebäude!I55</f>
         <v>2.0907165493471553</v>
       </c>
       <c r="AE13" t="s">
@@ -3360,7 +3271,7 @@
         <v>31</v>
       </c>
       <c r="AC14">
-        <f>H29*(D29/$D$36)*$F$2/Gebäude!I56</f>
+        <f>H30*(D30/$D$37)*$F$2/Gebäude!I56</f>
         <v>0</v>
       </c>
       <c r="AE14" t="s">
@@ -3449,7 +3360,7 @@
         <v>31</v>
       </c>
       <c r="AC15">
-        <f>H30*(D30/$D$36)*$F$2/Gebäude!I57</f>
+        <f>H31*(D31/$D$37)*$F$2/Gebäude!I57</f>
         <v>0</v>
       </c>
       <c r="AE15" t="s">
@@ -3538,7 +3449,7 @@
         <v>30</v>
       </c>
       <c r="AC16">
-        <f>H31*(D31/$D$36)*$F$2/Gebäude!I58</f>
+        <f>H32*(D32/$D$37)*$F$2/Gebäude!I58</f>
         <v>24.629688452901568</v>
       </c>
       <c r="AE16" t="s">
@@ -3627,7 +3538,7 @@
         <v>31</v>
       </c>
       <c r="AC17">
-        <f>H32*(D32/$D$36)*$F$2/Gebäude!I59</f>
+        <f>H33*(D33/$D$37)*$F$2/Gebäude!I59</f>
         <v>113.2895252340647</v>
       </c>
       <c r="AE17" t="s">
@@ -3716,7 +3627,7 @@
         <v>30</v>
       </c>
       <c r="AC18">
-        <f>H33*(D33/$D$36)*$F$2/Gebäude!I60</f>
+        <f>H34*(D34/$D$37)*$F$2/Gebäude!I60</f>
         <v>276.28548392783478</v>
       </c>
       <c r="AE18" t="s">
@@ -3805,7 +3716,7 @@
         <v>31</v>
       </c>
       <c r="AC19" s="4">
-        <f>H34*(D34/$D$36)*$F$2/Gebäude!I61</f>
+        <f>H35*(D35/$D$37)*$F$2/Gebäude!I61</f>
         <v>416.83354456285019</v>
       </c>
       <c r="AE19" s="4" t="s">
@@ -3843,7 +3754,7 @@
         <f t="shared" si="10"/>
         <v>3316.0228461359998</v>
       </c>
-      <c r="R20" s="23">
+      <c r="R20" s="16">
         <f>SUM(R8:R19)</f>
         <v>11226.772665108001</v>
       </c>
@@ -3875,704 +3786,1069 @@
         <v>20146.759367628903</v>
       </c>
     </row>
-    <row r="21" spans="2:32" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="2:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+    </row>
     <row r="22" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B22" s="2" t="s">
+      <c r="J22" s="2"/>
+      <c r="AA22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B23" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-    </row>
-    <row r="23" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="1">
-        <v>31</v>
-      </c>
-      <c r="D23" s="8">
-        <v>0.56732407424029996</v>
-      </c>
-      <c r="E23" s="8">
-        <v>19.168641979741</v>
-      </c>
-      <c r="F23" s="1">
-        <f t="shared" ref="F23:F34" si="11">$C$4*((E23+12)/32)*D23</f>
-        <v>10352.572367942394</v>
-      </c>
-      <c r="G23">
-        <f>F23-(F8+(0.5*R8)*Gebäude!I50)</f>
-        <v>9669.9067878173937</v>
-      </c>
-      <c r="H23">
-        <f>IF(G23&lt;0,0,G23)</f>
-        <v>9669.9067878173937</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="J23" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AA23" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K23" t="s">
-        <v>155</v>
-      </c>
-      <c r="L23" t="s">
-        <v>156</v>
-      </c>
-      <c r="M23" t="s">
-        <v>157</v>
-      </c>
-      <c r="N23" t="s">
-        <v>159</v>
-      </c>
-      <c r="O23" t="s">
-        <v>158</v>
-      </c>
-      <c r="P23" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>161</v>
+      <c r="AB23" s="2" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="1">
+        <v>31</v>
+      </c>
+      <c r="D24" s="7">
+        <v>0.56732407424029996</v>
+      </c>
+      <c r="E24" s="7">
+        <v>19.168641979741</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" ref="F24:F35" si="11">$C$4*((E24+12)/32)*D24</f>
+        <v>10352.572367942394</v>
+      </c>
+      <c r="G24">
+        <f>F24-(F8+(0.5*R8)*Gebäude!I50)</f>
+        <v>9669.9067878173937</v>
+      </c>
+      <c r="H24">
+        <f>IF(G24&lt;0,0,G24)</f>
+        <v>9669.9067878173937</v>
+      </c>
+      <c r="I24">
+        <f>AF8*Gebäude!I50</f>
+        <v>1824.8068659992102</v>
+      </c>
+      <c r="J24">
+        <f>I24/F24</f>
+        <v>0.17626603332422744</v>
+      </c>
+      <c r="K24" s="7">
+        <v>0.99366137766730001</v>
+      </c>
+      <c r="L24">
+        <f>1-K24*J24</f>
+        <v>0.82485125049109798</v>
+      </c>
+      <c r="M24">
+        <f>IF(L24&lt;=0,0,L24)</f>
+        <v>0.82485125049109798</v>
+      </c>
+      <c r="N24">
+        <f>D24*M24</f>
+        <v>0.46795797207081591</v>
+      </c>
+      <c r="O24">
+        <f>C24*24</f>
+        <v>744</v>
+      </c>
+      <c r="P24">
+        <f>(N24/0.05)*C24*24</f>
+        <v>6963.2146244137402</v>
+      </c>
+      <c r="Q24">
+        <f>IF(N24&gt;0.05,O24,P24)</f>
+        <v>744</v>
+      </c>
+      <c r="R24" s="7">
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <f>1-(10-R24)/22</f>
+        <v>0.59090909090909083</v>
+      </c>
+      <c r="T24">
+        <f>IF(Gebäude!B3=1,1,Bilanzierung!S24)</f>
+        <v>0.59090909090909083</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB24" s="20">
+        <f>F24*M24*Q24/1000</f>
+        <v>6353.2632040416711</v>
+      </c>
+    </row>
+    <row r="25" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C25" s="1">
         <v>28</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D25" s="7">
         <v>0.54121604949352997</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E25" s="7">
         <v>19.208641979741</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F25" s="1">
         <f t="shared" si="11"/>
         <v>9888.8256400439677</v>
       </c>
-      <c r="G24">
-        <f>F24-(F9+(0.5*R9)*Gebäude!I51)</f>
+      <c r="G25">
+        <f>F25-(F9+(0.5*R9)*Gebäude!I51)</f>
         <v>9227.7345415439668</v>
       </c>
-      <c r="H24">
-        <f t="shared" ref="H24:H34" si="12">IF(G24&lt;0,0,G24)</f>
+      <c r="H25">
+        <f t="shared" ref="H25:H35" si="12">IF(G25&lt;0,0,G25)</f>
         <v>9227.7345415439668</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K24">
-        <f>AF8*Gebäude!I50</f>
-        <v>1824.8068659992102</v>
-      </c>
-      <c r="L24">
-        <f>K24/F23</f>
-        <v>0.17626603332422744</v>
-      </c>
-      <c r="M24" s="25">
-        <v>0.99366137766730001</v>
-      </c>
-      <c r="N24">
-        <f>1-M24*L24</f>
-        <v>0.82485125049109798</v>
-      </c>
-      <c r="O24">
-        <f>IF(N24&lt;=0,0,N24)</f>
-        <v>0.82485125049109798</v>
-      </c>
-      <c r="P24">
-        <f>D23*O24</f>
-        <v>0.46795797207081591</v>
-      </c>
-      <c r="AA24" s="7"/>
-    </row>
-    <row r="25" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
+      <c r="I25">
+        <f>AF9*Gebäude!I51</f>
+        <v>1819.9885584688273</v>
+      </c>
+      <c r="J25">
+        <f>I25/F25</f>
+        <v>0.18404496395395392</v>
+      </c>
+      <c r="K25" s="7">
+        <v>0.99311685252322002</v>
+      </c>
+      <c r="L25">
+        <f t="shared" ref="L25:L35" si="13">1-K25*J25</f>
+        <v>0.81722184467529979</v>
+      </c>
+      <c r="M25">
+        <f t="shared" ref="M25:M35" si="14">IF(L25&lt;=0,0,L25)</f>
+        <v>0.81722184467529979</v>
+      </c>
+      <c r="N25">
+        <f>D25*M25</f>
+        <v>0.4422935783349809</v>
+      </c>
+      <c r="O25">
+        <f t="shared" ref="O25:O35" si="15">C25*24</f>
+        <v>672</v>
+      </c>
+      <c r="P25">
+        <f t="shared" ref="P25:P35" si="16">(N25/0.05)*C25*24</f>
+        <v>5944.4256928221439</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" ref="Q25:Q35" si="17">IF(N25&gt;0.05,O25,P25)</f>
+        <v>672</v>
+      </c>
+      <c r="R25" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="S25">
+        <f t="shared" ref="S25:S35" si="18">1-(10-R25)/22</f>
+        <v>0.63181818181818183</v>
+      </c>
+      <c r="T25">
+        <f>IF(Gebäude!B4=1,1,Bilanzierung!S25)</f>
+        <v>0.63181818181818183</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB25" s="20">
+        <f>F25*M25*Q25/1000</f>
+        <v>5430.6768305859778</v>
+      </c>
+    </row>
+    <row r="26" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C26" s="1">
         <v>31</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D26" s="7">
         <v>0.45721604949353001</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E26" s="7">
         <v>0</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F26" s="1">
         <f t="shared" si="11"/>
         <v>3212.1949456636321</v>
       </c>
-      <c r="G25">
-        <f>F25-(F10+(0.5*R10)*Gebäude!I52)</f>
+      <c r="G26">
+        <f>F26-(F10+(0.5*R10)*Gebäude!I52)</f>
         <v>2198.0499672886322</v>
       </c>
-      <c r="H25">
+      <c r="H26">
         <f t="shared" si="12"/>
         <v>2198.0499672886322</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K25">
-        <f>AF9*Gebäude!I51</f>
-        <v>1819.9885584688273</v>
-      </c>
-      <c r="L25">
-        <f t="shared" ref="L25:L35" si="13">K25/F24</f>
-        <v>0.18404496395395392</v>
-      </c>
-      <c r="M25" s="25">
-        <v>0.99311685252322002</v>
-      </c>
-      <c r="N25">
-        <f t="shared" ref="N25:N35" si="14">1-M25*L25</f>
-        <v>0.81722184467529979</v>
-      </c>
-      <c r="O25">
-        <f t="shared" ref="O25:O35" si="15">IF(N25&lt;=0,0,N25)</f>
-        <v>0.81722184467529979</v>
-      </c>
-      <c r="P25">
-        <f t="shared" ref="P25:P35" si="16">D24*O25</f>
-        <v>0.4422935783349809</v>
-      </c>
-    </row>
-    <row r="26" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
+      <c r="I26">
+        <f>AF10*Gebäude!I52</f>
+        <v>2039.921565466685</v>
+      </c>
+      <c r="J26">
+        <f>I26/F26</f>
+        <v>0.63505534376751283</v>
+      </c>
+      <c r="K26" s="7">
+        <v>0.88002952280601998</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="13"/>
+        <v>0.44113254886886266</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="14"/>
+        <v>0.44113254886886266</v>
+      </c>
+      <c r="N26">
+        <f>D26*M26</f>
+        <v>0.20169288129683297</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="15"/>
+        <v>744</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="16"/>
+        <v>3001.1900736968746</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="17"/>
+        <v>744</v>
+      </c>
+      <c r="R26" s="7">
+        <v>4.7</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="18"/>
+        <v>0.75909090909090904</v>
+      </c>
+      <c r="T26">
+        <f>IF(Gebäude!B5=1,1,Bilanzierung!S26)</f>
+        <v>0.75909090909090904</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB26" s="20">
+        <f>F26*M26*Q26/1000</f>
+        <v>1054.2507854201413</v>
+      </c>
+    </row>
+    <row r="27" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C27" s="1">
         <v>30</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D27" s="7">
         <v>0.32310802474676997</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E27" s="7">
         <v>19.525401237337999</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F27" s="1">
         <f t="shared" si="11"/>
         <v>5963.5868516620267</v>
       </c>
-      <c r="G26">
-        <f>F26-(F11+(0.5*R11)*Gebäude!I53)</f>
+      <c r="G27">
+        <f>F27-(F11+(0.5*R11)*Gebäude!I53)</f>
         <v>4514.8736737870267</v>
       </c>
-      <c r="H26">
+      <c r="H27">
         <f t="shared" si="12"/>
         <v>4514.8736737870267</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="K26">
-        <f>AF10*Gebäude!I52</f>
-        <v>2039.921565466685</v>
-      </c>
-      <c r="L26">
+      <c r="I27">
+        <f>AF11*Gebäude!I53</f>
+        <v>2983.5729970125681</v>
+      </c>
+      <c r="J27">
+        <f>I27/F27</f>
+        <v>0.50029840618168553</v>
+      </c>
+      <c r="K27" s="7">
+        <v>0.92689854189822996</v>
+      </c>
+      <c r="L27">
         <f t="shared" si="13"/>
-        <v>0.63505534376751283</v>
-      </c>
-      <c r="M26" s="25">
-        <v>0.88002952280601998</v>
-      </c>
-      <c r="N26">
+        <v>0.5362741367961873</v>
+      </c>
+      <c r="M27">
         <f t="shared" si="14"/>
-        <v>0.44113254886886266</v>
-      </c>
-      <c r="O26">
+        <v>0.5362741367961873</v>
+      </c>
+      <c r="N27">
+        <f>D27*M27</f>
+        <v>0.1732744770629952</v>
+      </c>
+      <c r="O27">
         <f t="shared" si="15"/>
-        <v>0.44113254886886266</v>
-      </c>
-      <c r="P26">
+        <v>720</v>
+      </c>
+      <c r="P27">
         <f t="shared" si="16"/>
-        <v>0.20169288129683297</v>
-      </c>
-    </row>
-    <row r="27" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
+        <v>2495.1524697071309</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="17"/>
+        <v>720</v>
+      </c>
+      <c r="R27" s="7">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="18"/>
+        <v>0.96363636363636362</v>
+      </c>
+      <c r="T27">
+        <f>IF(Gebäude!B6=1,1,Bilanzierung!S27)</f>
+        <v>0.96363636363636362</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB27" s="20">
+        <f>F27*M27*Q27/1000</f>
+        <v>2302.6445215805848</v>
+      </c>
+    </row>
+    <row r="28" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C28" s="1">
         <v>31</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D28" s="7">
         <v>0.17610802474677001</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E28" s="7">
         <v>19.742160494935</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F28" s="1">
         <f t="shared" si="11"/>
         <v>3272.7649144272054</v>
       </c>
-      <c r="G27">
-        <f>F27-(F12+(0.5*R12)*Gebäude!I54)</f>
+      <c r="G28">
+        <f>F28-(F12+(0.5*R12)*Gebäude!I54)</f>
         <v>1763.6812418022057</v>
       </c>
-      <c r="H27">
+      <c r="H28">
         <f t="shared" si="12"/>
         <v>1763.6812418022057</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K27">
-        <f>AF11*Gebäude!I53</f>
-        <v>2983.5729970125681</v>
-      </c>
-      <c r="L27">
+      <c r="I28">
+        <f>AF12*Gebäude!I54</f>
+        <v>2960.3998806143359</v>
+      </c>
+      <c r="J28">
+        <f>I28/F28</f>
+        <v>0.90455622631620047</v>
+      </c>
+      <c r="K28" s="7">
+        <v>0.77826863399984003</v>
+      </c>
+      <c r="L28">
         <f t="shared" si="13"/>
-        <v>0.50029840618168553</v>
-      </c>
-      <c r="M27" s="25">
-        <v>0.92689854189822996</v>
-      </c>
-      <c r="N27">
+        <v>0.29601226136884051</v>
+      </c>
+      <c r="M28">
         <f t="shared" si="14"/>
-        <v>0.5362741367961873</v>
-      </c>
-      <c r="O27">
+        <v>0.29601226136884051</v>
+      </c>
+      <c r="N28">
+        <f>D28*M28</f>
+        <v>5.2130134650491114E-2</v>
+      </c>
+      <c r="O28">
         <f t="shared" si="15"/>
-        <v>0.5362741367961873</v>
-      </c>
-      <c r="P27">
+        <v>744</v>
+      </c>
+      <c r="P28">
         <f t="shared" si="16"/>
-        <v>0.1732744770629952</v>
-      </c>
-    </row>
-    <row r="28" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
+        <v>775.69640359930781</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="17"/>
+        <v>744</v>
+      </c>
+      <c r="R28" s="7">
+        <v>14.1</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="18"/>
+        <v>1.1863636363636363</v>
+      </c>
+      <c r="T28">
+        <f>IF(Gebäude!B7=1,1,Bilanzierung!S28)</f>
+        <v>1.1863636363636363</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB28" s="20">
+        <f>F28*M28*Q28/1000</f>
+        <v>720.77123617665859</v>
+      </c>
+    </row>
+    <row r="29" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C29" s="1">
         <v>30</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D29" s="7">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E29" s="7">
         <v>19.852160494934999</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F29" s="1">
         <f t="shared" si="11"/>
         <v>1846.1767249312081</v>
       </c>
-      <c r="G28">
-        <f>F28-(F13+(0.5*R13)*Gebäude!I55)</f>
+      <c r="G29">
+        <f>F29-(F13+(0.5*R13)*Gebäude!I55)</f>
         <v>293.47716455620798</v>
       </c>
-      <c r="H28">
+      <c r="H29">
         <f t="shared" si="12"/>
         <v>293.47716455620798</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K28">
-        <f>AF12*Gebäude!I54</f>
-        <v>2960.3998806143359</v>
-      </c>
-      <c r="L28">
+      <c r="I29">
+        <f>AF13*Gebäude!I55</f>
+        <v>3048.6532362009584</v>
+      </c>
+      <c r="J29">
+        <f>I29/F29</f>
+        <v>1.6513333718442131</v>
+      </c>
+      <c r="K29" s="7">
+        <v>0.54016665703894995</v>
+      </c>
+      <c r="L29">
         <f t="shared" si="13"/>
-        <v>0.90455622631620047</v>
-      </c>
-      <c r="M28" s="25">
-        <v>0.77826863399984003</v>
-      </c>
-      <c r="N28">
+        <v>0.10800477287405408</v>
+      </c>
+      <c r="M29">
         <f t="shared" si="14"/>
-        <v>0.29601226136884051</v>
-      </c>
-      <c r="O28">
+        <v>0.10800477287405408</v>
+      </c>
+      <c r="N29">
+        <f>D29*M29</f>
+        <v>1.0692472514531355E-2</v>
+      </c>
+      <c r="O29">
         <f t="shared" si="15"/>
-        <v>0.29601226136884051</v>
-      </c>
-      <c r="P28">
+        <v>720</v>
+      </c>
+      <c r="P29">
         <f t="shared" si="16"/>
-        <v>5.2130134650491114E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
+        <v>153.9716042092515</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="17"/>
+        <v>153.9716042092515</v>
+      </c>
+      <c r="R29" s="7">
+        <v>16.7</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="18"/>
+        <v>1.3045454545454545</v>
+      </c>
+      <c r="T29">
+        <f>IF(Gebäude!B8=1,1,Bilanzierung!S29)</f>
+        <v>1.3045454545454545</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB29" s="20">
+        <f>F29*M29*Q29/1000</f>
+        <v>30.701306266488476</v>
+      </c>
+    </row>
+    <row r="30" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C30" s="1">
         <v>31</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D30" s="7">
         <v>0.03</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E30" s="7">
         <v>19.96</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F30" s="1">
         <f t="shared" si="11"/>
         <v>561.34157242036201</v>
       </c>
-      <c r="G29">
-        <f>F29-(F14+(0.5*R14)*Gebäude!I56)</f>
+      <c r="G30">
+        <f>F30-(F14+(0.5*R14)*Gebäude!I56)</f>
         <v>-901.40430870463786</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K29">
-        <f>AF13*Gebäude!I55</f>
-        <v>3048.6532362009584</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="13"/>
-        <v>1.6513333718442131</v>
-      </c>
-      <c r="M29" s="25">
-        <v>0.54016665703894995</v>
-      </c>
-      <c r="N29">
-        <f t="shared" si="14"/>
-        <v>0.10800477287405408</v>
-      </c>
-      <c r="O29">
-        <f t="shared" si="15"/>
-        <v>0.10800477287405408</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="16"/>
-        <v>1.0692472514531355E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="1">
-        <v>31</v>
-      </c>
-      <c r="D30" s="8">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="E30" s="8">
-        <v>19.940000000000001</v>
-      </c>
-      <c r="F30" s="1">
-        <f t="shared" si="11"/>
-        <v>785.38641277687452</v>
-      </c>
-      <c r="G30">
-        <f>F30-(F15+(0.5*R15)*Gebäude!I57)</f>
-        <v>-567.44403772312535</v>
       </c>
       <c r="H30">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="J30" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="K30">
+      <c r="I30">
         <f>AF14*Gebäude!I56</f>
         <v>2836.6821047157532</v>
       </c>
+      <c r="J30">
+        <f>I30/F30</f>
+        <v>5.0533975106897957</v>
+      </c>
+      <c r="K30" s="7">
+        <v>0.19618448463655</v>
+      </c>
       <c r="L30">
         <f t="shared" si="13"/>
-        <v>5.0533975106897957</v>
-      </c>
-      <c r="M30" s="25">
-        <v>0.19618448463655</v>
-      </c>
-      <c r="N30">
+        <v>8.6018137016977692E-3</v>
+      </c>
+      <c r="M30">
         <f t="shared" si="14"/>
         <v>8.6018137016977692E-3</v>
       </c>
+      <c r="N30">
+        <f>D30*M30</f>
+        <v>2.5805441105093306E-4</v>
+      </c>
       <c r="O30">
         <f t="shared" si="15"/>
-        <v>8.6018137016977692E-3</v>
+        <v>744</v>
       </c>
       <c r="P30">
         <f t="shared" si="16"/>
-        <v>2.5805441105093306E-4</v>
+        <v>3.8398496364378838</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="17"/>
+        <v>3.8398496364378838</v>
+      </c>
+      <c r="R30" s="7">
+        <v>19</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="18"/>
+        <v>1.4090909090909092</v>
+      </c>
+      <c r="T30">
+        <f>IF(Gebäude!B9=1,1,Bilanzierung!S30)</f>
+        <v>1.4090909090909092</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB30" s="20">
+        <f>F30*M30*Q30/1000</f>
+        <v>1.8540927576451427E-2</v>
       </c>
     </row>
     <row r="31" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C31" s="1">
-        <v>30</v>
-      </c>
-      <c r="D31" s="8">
-        <v>0.17010802474677</v>
-      </c>
-      <c r="E31" s="8">
-        <v>19.752160494935001</v>
+        <v>31</v>
+      </c>
+      <c r="D31" s="7">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="E31" s="7">
+        <v>19.940000000000001</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" si="11"/>
-        <v>3162.2577402046868</v>
+        <v>785.38641277687452</v>
       </c>
       <c r="G31">
-        <f>F31-(F16+(0.5*R16)*Gebäude!I58)</f>
-        <v>2012.0949394546869</v>
+        <f>F31-(F15+(0.5*R15)*Gebäude!I57)</f>
+        <v>-567.44403772312535</v>
       </c>
       <c r="H31">
         <f t="shared" si="12"/>
-        <v>2012.0949394546869</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="I31">
         <f>AF15*Gebäude!I57</f>
         <v>2616.8512434657532</v>
       </c>
+      <c r="J31">
+        <f>I31/F31</f>
+        <v>3.3319283360319494</v>
+      </c>
+      <c r="K31" s="7">
+        <v>0.29344573311743999</v>
+      </c>
       <c r="L31">
         <f t="shared" si="13"/>
-        <v>3.3319283360319494</v>
-      </c>
-      <c r="M31" s="25">
-        <v>0.29344573311743999</v>
-      </c>
-      <c r="N31">
+        <v>2.22598467383327E-2</v>
+      </c>
+      <c r="M31">
         <f t="shared" si="14"/>
         <v>2.22598467383327E-2</v>
       </c>
+      <c r="N31">
+        <f>D31*M31</f>
+        <v>9.3491356300997349E-4</v>
+      </c>
       <c r="O31">
         <f t="shared" si="15"/>
-        <v>2.22598467383327E-2</v>
+        <v>744</v>
       </c>
       <c r="P31">
         <f t="shared" si="16"/>
-        <v>9.3491356300997349E-4</v>
+        <v>13.911513817588403</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="17"/>
+        <v>13.911513817588403</v>
+      </c>
+      <c r="R31" s="7">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="18"/>
+        <v>1.3909090909090911</v>
+      </c>
+      <c r="T31">
+        <f>IF(Gebäude!B10=1,1,Bilanzierung!S31)</f>
+        <v>1.3909090909090911</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB31" s="20">
+        <f>F31*M31*Q31/1000</f>
+        <v>0.24320916963573855</v>
       </c>
     </row>
     <row r="32" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C32" s="1">
-        <v>31</v>
-      </c>
-      <c r="D32" s="8">
-        <v>0.31410802474677002</v>
-      </c>
-      <c r="E32" s="8">
-        <v>19.535401237338</v>
+        <v>30</v>
+      </c>
+      <c r="D32" s="7">
+        <v>0.17010802474677</v>
+      </c>
+      <c r="E32" s="7">
+        <v>19.752160494935001</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" si="11"/>
-        <v>5799.3133370703099</v>
+        <v>3162.2577402046868</v>
       </c>
       <c r="G32">
-        <f>F32-(F17+(0.5*R17)*Gebäude!I59)</f>
-        <v>4850.4791041953094</v>
+        <f>F32-(F16+(0.5*R16)*Gebäude!I58)</f>
+        <v>2012.0949394546869</v>
       </c>
       <c r="H32">
         <f t="shared" si="12"/>
-        <v>4850.4791041953094</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K32">
+        <v>2012.0949394546869</v>
+      </c>
+      <c r="I32">
         <f>AF16*Gebäude!I58</f>
         <v>2274.8838445947831</v>
       </c>
+      <c r="J32">
+        <f>I32/F32</f>
+        <v>0.7193859677129083</v>
+      </c>
+      <c r="K32" s="7">
+        <v>0.84863333226908999</v>
+      </c>
       <c r="L32">
         <f t="shared" si="13"/>
-        <v>0.7193859677129083</v>
-      </c>
-      <c r="M32" s="25">
-        <v>0.84863333226908999</v>
-      </c>
-      <c r="N32">
+        <v>0.38950508903217063</v>
+      </c>
+      <c r="M32">
         <f t="shared" si="14"/>
         <v>0.38950508903217063</v>
       </c>
+      <c r="N32">
+        <f>D32*M32</f>
+        <v>6.6257941324077335E-2</v>
+      </c>
       <c r="O32">
         <f t="shared" si="15"/>
-        <v>0.38950508903217063</v>
+        <v>720</v>
       </c>
       <c r="P32">
         <f t="shared" si="16"/>
-        <v>6.6257941324077335E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
+        <v>954.11435506671341</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="17"/>
+        <v>720</v>
+      </c>
+      <c r="R32" s="7">
+        <v>14.3</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="18"/>
+        <v>1.1954545454545455</v>
+      </c>
+      <c r="T32">
+        <f>IF(Gebäude!B11=1,1,Bilanzierung!S32)</f>
+        <v>1.1954545454545455</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB32" s="20">
+        <f>F32*M32*Q32/1000</f>
+        <v>886.83514750158997</v>
+      </c>
+    </row>
+    <row r="33" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" s="1">
-        <v>30</v>
-      </c>
-      <c r="D33" s="8">
-        <v>0.47521604949353002</v>
-      </c>
-      <c r="E33" s="8">
-        <v>19.306481484806</v>
+        <v>31</v>
+      </c>
+      <c r="D33" s="7">
+        <v>0.31410802474677002</v>
+      </c>
+      <c r="E33" s="7">
+        <v>19.535401237338</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" si="11"/>
-        <v>8710.1280840494492</v>
+        <v>5799.3133370703099</v>
       </c>
       <c r="G33">
-        <f>F33-(F18+(0.5*R18)*Gebäude!I60)</f>
-        <v>8079.4411151744489</v>
+        <f>F33-(F17+(0.5*R17)*Gebäude!I59)</f>
+        <v>4850.4791041953094</v>
       </c>
       <c r="H33">
         <f t="shared" si="12"/>
-        <v>8079.4411151744489</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K33">
+        <v>4850.4791041953094</v>
+      </c>
+      <c r="I33">
         <f>AF17*Gebäude!I59</f>
         <v>1961.1296754658406</v>
       </c>
+      <c r="J33">
+        <f>I33/F33</f>
+        <v>0.3381658416229949</v>
+      </c>
+      <c r="K33" s="7">
+        <v>0.96960351484294005</v>
+      </c>
       <c r="L33">
         <f t="shared" si="13"/>
-        <v>0.3381658416229949</v>
-      </c>
-      <c r="M33" s="25">
-        <v>0.96960351484294005</v>
-      </c>
-      <c r="N33">
+        <v>0.67211321136252322</v>
+      </c>
+      <c r="M33">
         <f t="shared" si="14"/>
         <v>0.67211321136252322</v>
       </c>
+      <c r="N33">
+        <f>D33*M33</f>
+        <v>0.21111615322729052</v>
+      </c>
       <c r="O33">
         <f t="shared" si="15"/>
-        <v>0.67211321136252322</v>
+        <v>744</v>
       </c>
       <c r="P33">
         <f t="shared" si="16"/>
-        <v>0.21111615322729052</v>
-      </c>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.2">
+        <v>3141.4083600220829</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="17"/>
+        <v>744</v>
+      </c>
+      <c r="R33" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="18"/>
+        <v>0.97727272727272729</v>
+      </c>
+      <c r="T33">
+        <f>IF(Gebäude!B12=1,1,Bilanzierung!S33)</f>
+        <v>0.97727272727272729</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB33" s="20">
+        <f>F33*M33*Q33/1000</f>
+        <v>2899.9595623428227</v>
+      </c>
+    </row>
+    <row r="34" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C34" s="1">
-        <v>31</v>
-      </c>
-      <c r="D34" s="8">
-        <v>0.57032407424029996</v>
-      </c>
-      <c r="E34" s="8">
-        <v>19.159722227208999</v>
+        <v>30</v>
+      </c>
+      <c r="D34" s="7">
+        <v>0.47521604949353002</v>
+      </c>
+      <c r="E34" s="7">
+        <v>19.306481484806</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" si="11"/>
-        <v>10404.338257532285</v>
+        <v>8710.1280840494492</v>
       </c>
       <c r="G34">
-        <f>F34-(F19+(0.5*R19)*Gebäude!I61)</f>
-        <v>9829.1252726572857</v>
+        <f>F34-(F18+(0.5*R18)*Gebäude!I60)</f>
+        <v>8079.4411151744489</v>
       </c>
       <c r="H34">
         <f t="shared" si="12"/>
-        <v>9829.1252726572857</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K34">
+        <v>8079.4411151744489</v>
+      </c>
+      <c r="I34">
         <f>AF18*Gebäude!I60</f>
         <v>1585.4541190044131</v>
       </c>
+      <c r="J34">
+        <f>I34/F34</f>
+        <v>0.1820242025955737</v>
+      </c>
+      <c r="K34" s="7">
+        <v>0.99325830581830998</v>
+      </c>
       <c r="L34">
         <f t="shared" si="13"/>
-        <v>0.1820242025955737</v>
-      </c>
-      <c r="M34" s="25">
-        <v>0.99325830581830998</v>
-      </c>
-      <c r="N34">
+        <v>0.81920294891199164</v>
+      </c>
+      <c r="M34">
         <f t="shared" si="14"/>
         <v>0.81920294891199164</v>
       </c>
+      <c r="N34">
+        <f>D34*M34</f>
+        <v>0.38929838911540676</v>
+      </c>
       <c r="O34">
         <f t="shared" si="15"/>
-        <v>0.81920294891199164</v>
+        <v>720</v>
       </c>
       <c r="P34">
         <f t="shared" si="16"/>
-        <v>0.38929838911540676</v>
-      </c>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="J35" s="1" t="s">
+        <v>5605.8968032618577</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="17"/>
+        <v>720</v>
+      </c>
+      <c r="R34" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="18"/>
+        <v>0.73181818181818181</v>
+      </c>
+      <c r="T34">
+        <f>IF(Gebäude!B13=1,1,Bilanzierung!S34)</f>
+        <v>0.73181818181818181</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB34" s="20">
+        <f>F34*M34*Q34/1000</f>
+        <v>5137.461080535214</v>
+      </c>
+    </row>
+    <row r="35" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K35">
+      <c r="C35" s="1">
+        <v>31</v>
+      </c>
+      <c r="D35" s="7">
+        <v>0.57032407424029996</v>
+      </c>
+      <c r="E35" s="7">
+        <v>19.159722227208999</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="11"/>
+        <v>10404.338257532285</v>
+      </c>
+      <c r="G35">
+        <f>F35-(F19+(0.5*R19)*Gebäude!I61)</f>
+        <v>9829.1252726572857</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="12"/>
+        <v>9829.1252726572857</v>
+      </c>
+      <c r="I35">
         <f>AF19*Gebäude!I61</f>
         <v>1621.8764527572184</v>
       </c>
+      <c r="J35">
+        <f>I35/F35</f>
+        <v>0.15588463318011128</v>
+      </c>
+      <c r="K35" s="7">
+        <v>0.99508807567738999</v>
+      </c>
       <c r="L35">
         <f t="shared" si="13"/>
-        <v>0.15588463318011128</v>
-      </c>
-      <c r="M35" s="25">
-        <v>0.99508807567738999</v>
-      </c>
-      <c r="N35">
+        <v>0.8448810603411272</v>
+      </c>
+      <c r="M35">
         <f t="shared" si="14"/>
         <v>0.8448810603411272</v>
       </c>
+      <c r="N35">
+        <f>D35*M35</f>
+        <v>0.48185600858221639</v>
+      </c>
       <c r="O35">
         <f t="shared" si="15"/>
-        <v>0.8448810603411272</v>
+        <v>744</v>
       </c>
       <c r="P35">
         <f t="shared" si="16"/>
-        <v>0.48185600858221639</v>
-      </c>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B36" s="24" t="s">
+        <v>7170.0174077033789</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="17"/>
+        <v>744</v>
+      </c>
+      <c r="R35" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="18"/>
+        <v>0.58636363636363642</v>
+      </c>
+      <c r="T35">
+        <f>IF(Gebäude!B14=1,1,Bilanzierung!S35)</f>
+        <v>0.58636363636363642</v>
+      </c>
+      <c r="AA35" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB35" s="21">
+        <f>F35*M35*Q35/1000</f>
+        <v>6540.0786843436945</v>
+      </c>
+    </row>
+    <row r="36" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="AA36" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB36" s="23">
+        <f>SUM(AB24:AB35)</f>
+        <v>31356.904108892053</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="37" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B37" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D36">
-        <f>MAX(D23:D34)</f>
+      <c r="D37">
+        <f>MAX(D24:D35)</f>
         <v>0.57032407424029996</v>
       </c>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+      <c r="M37" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="N37">
+        <f>SUM(N24:N35)</f>
+        <v>2.4977629761536995</v>
+      </c>
+    </row>
+    <row r="39" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
         <v>78</v>
       </c>
-      <c r="K38" s="7"/>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
+      <c r="K39" s="6"/>
+    </row>
+    <row r="41" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="R41" s="6" t="s">
+        <v>168</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -4582,152 +4858,172 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9336C9-D30B-3E41-B0AD-8BF2B56C5439}">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575576D5-D868-1A43-98B7-3D2B5532C56B}">
+  <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1048576"/>
+      <selection activeCell="B2" sqref="B2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="5">
-        <v>31</v>
-      </c>
-      <c r="C1" s="5">
-        <v>0.56732407424029996</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="5">
-        <v>28</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0.54121604949352997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="5">
-        <v>31</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0.45721604949353001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="5">
-        <v>30</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0.32310802474676997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="5">
-        <v>31</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0.17610802474677001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="5">
-        <v>30</v>
-      </c>
-      <c r="C6" s="5">
-        <v>9.9000000000000005E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="5">
-        <v>31</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="5">
-        <v>31</v>
-      </c>
-      <c r="C8" s="5">
-        <v>4.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="5">
-        <v>30</v>
-      </c>
-      <c r="C9" s="5">
-        <v>0.17010802474677</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="5">
-        <v>31</v>
-      </c>
-      <c r="C10" s="5">
-        <v>0.31410802474677002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="5">
-        <v>30</v>
-      </c>
-      <c r="C11" s="5">
-        <v>0.47521604949353002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="5">
-        <v>31</v>
-      </c>
-      <c r="C12" s="5">
-        <v>0.57032407424029996</v>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7">
+        <f>IF(C5="innerhalb",IF(C6="Ja",1.554,0.647),IF(C6="Ja",0.815,0.335))</f>
+        <v>1.554</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8">
+        <f>IF(C6="Ja",1.321,0.451)</f>
+        <v>1.321</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="2">
+        <f>IF(C3="Ja",IF(C4="Ja",C7,C8),0.193)</f>
+        <v>1.321</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>174</v>
+      </c>
+      <c r="C20" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>138</v>
+      </c>
+      <c r="C22" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>175</v>
+      </c>
+      <c r="C25" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>175</v>
+      </c>
+      <c r="C26" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>175</v>
+      </c>
+      <c r="C27" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>175</v>
+      </c>
+      <c r="C28" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Testberechnungen auf aktuellem Stand
</commit_message>
<xml_diff>
--- a/din18599/Testberechnungen.xlsx
+++ b/din18599/Testberechnungen.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wagesve/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wagesve/Dev/Sites/enon/din18599/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D446FFF0-634D-8246-984F-F0B1822B82C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C740E7-5BE6-7D4F-B17D-562C8632FEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{7CF02650-DC02-AA49-AC3A-4487EF2FF614}"/>
   </bookViews>
   <sheets>
     <sheet name="Gebäude" sheetId="1" r:id="rId1"/>
     <sheet name="Dach" sheetId="2" r:id="rId2"/>
-    <sheet name="Wärmequellen" sheetId="3" r:id="rId3"/>
-    <sheet name="Tabelle1" sheetId="4" r:id="rId4"/>
+    <sheet name="Bilanzierung" sheetId="3" r:id="rId3"/>
+    <sheet name="Heizung" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="211">
   <si>
     <t>Haus Rechteckig</t>
   </si>
@@ -567,17 +567,140 @@
     <t>flna</t>
   </si>
   <si>
-    <t>1 - ( ( 10 - $this-&gt;monatsdaten-&gt;temperatur( $monat ) ) / 22 );</t>
-  </si>
-  <si>
     <t xml:space="preserve">ithrl </t>
+  </si>
+  <si>
+    <t>Übergabesystem</t>
+  </si>
+  <si>
+    <t>elektroheizungsflaechen/heizkoerper/flaechenheizung</t>
+  </si>
+  <si>
+    <t>flaechenheizung</t>
+  </si>
+  <si>
+    <t>Werte aus Gebäudedaten</t>
+  </si>
+  <si>
+    <t>Aufwandszahl für freie Heizflaechen</t>
+  </si>
+  <si>
+    <t>Elektroheizungsflächen</t>
+  </si>
+  <si>
+    <t>Heizkörper</t>
+  </si>
+  <si>
+    <t>Flächenheizung</t>
+  </si>
+  <si>
+    <t>Auslegungstemperaturen Heizung</t>
+  </si>
+  <si>
+    <t>Auslegungstemperaturen Heizkörper</t>
+  </si>
+  <si>
+    <t>Übertemperatur Heizkörper</t>
+  </si>
+  <si>
+    <t>35/28</t>
+  </si>
+  <si>
+    <t>Typ der Flächenheizung</t>
+  </si>
+  <si>
+    <t>fussbodenheizung/wandheizung/deckenheizung</t>
+  </si>
+  <si>
+    <t>fussbodenheizung</t>
+  </si>
+  <si>
+    <t>Zwischenwert Flächenheizungstyp</t>
+  </si>
+  <si>
+    <t>Zwischenwert Mindestdämmung</t>
+  </si>
+  <si>
+    <t>Mindestdämmung vorhanden (Flächenheizung)</t>
+  </si>
+  <si>
+    <t>ehce</t>
+  </si>
+  <si>
+    <t>ßhce</t>
+  </si>
+  <si>
+    <t>Thm</t>
+  </si>
+  <si>
+    <t>$Φh,max</t>
+  </si>
+  <si>
+    <t>qhce</t>
+  </si>
+  <si>
+    <t>ehd</t>
+  </si>
+  <si>
+    <t>ausserhalb</t>
+  </si>
+  <si>
+    <t>EFH</t>
+  </si>
+  <si>
+    <t>Gebäude</t>
+  </si>
+  <si>
+    <t>Auslegunstemperaturen</t>
+  </si>
+  <si>
+    <t>90/70</t>
+  </si>
+  <si>
+    <t>70/55</t>
+  </si>
+  <si>
+    <t>55/45</t>
+  </si>
+  <si>
+    <t>MFH</t>
+  </si>
+  <si>
+    <t>Haus</t>
+  </si>
+  <si>
+    <t>Standort der Heizungsanlage</t>
+  </si>
+  <si>
+    <t>ehd0</t>
+  </si>
+  <si>
+    <t>ßhd</t>
+  </si>
+  <si>
+    <t>Wert für Tests manuell aus oberer Tabelle ermitteln</t>
+  </si>
+  <si>
+    <t>fßd</t>
+  </si>
+  <si>
+    <t>Interpolierter Wert aus Tabelle 32 übernommen aus Skript</t>
+  </si>
+  <si>
+    <t>ehd1</t>
+  </si>
+  <si>
+    <t>ehd korr</t>
+  </si>
+  <si>
+    <t>iht_rl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -605,12 +728,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -803,24 +920,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -830,11 +946,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1149,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D0A30B-5A9B-F949-B5FE-8B73CA8912C0}">
-  <dimension ref="A1:P78"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1962,16 +2080,16 @@
       <c r="A40" t="s">
         <v>83</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="7">
         <v>0.47099999999999997</v>
       </c>
-      <c r="C40" s="6"/>
+      <c r="C40" s="5"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>84</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="7">
         <v>1.0660000000000001</v>
       </c>
       <c r="G41" s="2" t="s">
@@ -1982,7 +2100,7 @@
       <c r="A42" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="7">
         <v>0.79</v>
       </c>
       <c r="G42" t="s">
@@ -2056,7 +2174,7 @@
       <c r="B48" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="7"/>
+      <c r="C48" s="6"/>
       <c r="G48" s="2" t="s">
         <v>148</v>
       </c>
@@ -2113,7 +2231,7 @@
       <c r="A52" t="s">
         <v>99</v>
       </c>
-      <c r="B52" s="8">
+      <c r="B52" s="7">
         <v>0.79</v>
       </c>
       <c r="G52" s="1" t="s">
@@ -2208,7 +2326,7 @@
         <f>(B37+B43-0.5*B15*0.34*(B52-B51))*32</f>
         <v>15427.801052661227</v>
       </c>
-      <c r="C58" s="7"/>
+      <c r="C58" s="6"/>
       <c r="G58" s="1" t="s">
         <v>63</v>
       </c>
@@ -2228,7 +2346,7 @@
         <f>(B43-0.5*B15*0.34*(B52-B51))*32</f>
         <v>3512.606202950401</v>
       </c>
-      <c r="C59" s="7"/>
+      <c r="C59" s="6"/>
       <c r="G59" s="1" t="s">
         <v>64</v>
       </c>
@@ -2248,7 +2366,7 @@
         <f>IF(B49="Ja",B58,B59)</f>
         <v>3512.606202950401</v>
       </c>
-      <c r="C60" s="7"/>
+      <c r="C60" s="6"/>
       <c r="G60" s="1" t="s">
         <v>65</v>
       </c>
@@ -2303,7 +2421,7 @@
       <c r="A69" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B69" s="8">
+      <c r="B69" s="7">
         <v>8.5</v>
       </c>
       <c r="C69" t="s">
@@ -2355,28 +2473,74 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>169</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C76" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>177</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>178</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>181</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C79" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>186</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>143</v>
       </c>
-      <c r="B76">
+      <c r="B82">
         <f>IF(B74="innerhalb",IF(B75="Ja",1.554,0.647),IF(B75="Ja",0.815,0.335))</f>
         <v>1.554</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>144</v>
       </c>
-      <c r="B77">
+      <c r="B83">
         <f>IF(B75="Ja",1.321,0.451)</f>
         <v>1.321</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="2" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B78" s="2">
-        <f>IF(B72="Ja",IF(B73="Ja",B76,B77),0.193)</f>
+      <c r="B84" s="2">
+        <f>IF(B72="Ja",IF(B73="Ja",B82,B83),0.193)</f>
         <v>1.321</v>
       </c>
     </row>
@@ -2390,7 +2554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CF28B4-6980-5D4B-8184-D8E1A3E7B562}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="D8" zoomScale="150" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -2551,8 +2715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A340B5-F068-DF4D-BA05-F7AD24B208A4}">
   <dimension ref="B2:AF40"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Y26" sqref="Y26"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S38" sqref="S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2587,7 +2751,7 @@
       <c r="E2" t="s">
         <v>150</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="G2" t="s">
@@ -2609,16 +2773,16 @@
         <f>Gebäude!B34</f>
         <v>0.78</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="10"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="9"/>
     </row>
     <row r="4" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
@@ -2638,8 +2802,8 @@
         <f>0.9*1*0.9*0.7*I3</f>
         <v>0.44225999999999999</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="15" t="s">
+      <c r="J4" s="6"/>
+      <c r="K4" s="14" t="s">
         <v>118</v>
       </c>
       <c r="L4" s="4">
@@ -2663,7 +2827,7 @@
       <c r="Q4" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="R4" s="16">
+      <c r="R4" s="15">
         <f>Gebäude!M14</f>
         <v>11.9625</v>
       </c>
@@ -2678,7 +2842,7 @@
         <v>147</v>
       </c>
       <c r="Y4">
-        <f>Gebäude!B78</f>
+        <f>Gebäude!B84</f>
         <v>1.321</v>
       </c>
     </row>
@@ -2690,19 +2854,19 @@
       <c r="H6" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="17" t="s">
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="19"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="18"/>
       <c r="T6" s="2" t="s">
         <v>133</v>
       </c>
@@ -2735,43 +2899,43 @@
       <c r="I7" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="L7" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="M7" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="O7" s="21" t="s">
+      <c r="O7" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="P7" s="21" t="s">
+      <c r="P7" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="Q7" s="21" t="s">
+      <c r="Q7" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="R7" s="22" t="s">
+      <c r="R7" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="T7" s="2" t="s">
+      <c r="T7" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="U7" s="2" t="s">
+      <c r="U7" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="V7" s="2" t="s">
+      <c r="V7" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="W7" s="11" t="s">
         <v>135</v>
       </c>
       <c r="AA7" s="2" t="s">
@@ -2904,7 +3068,7 @@
       <c r="L9">
         <v>47</v>
       </c>
-      <c r="M9" s="14">
+      <c r="M9" s="13">
         <v>24</v>
       </c>
       <c r="N9">
@@ -3876,7 +4040,7 @@
         <f t="shared" si="10"/>
         <v>3316.0228461359998</v>
       </c>
-      <c r="R20" s="23">
+      <c r="R20" s="22">
         <f>SUM(R8:R19)</f>
         <v>11226.772665108001</v>
       </c>
@@ -3912,73 +4076,72 @@
     <row r="22" spans="2:32" x14ac:dyDescent="0.2">
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
-      <c r="AA22" s="12" t="s">
+      <c r="AA22" s="11" t="s">
         <v>163</v>
       </c>
       <c r="AB22" s="4"/>
     </row>
     <row r="23" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="H23" s="12" t="s">
+      <c r="H23" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="I23" s="12" t="s">
+      <c r="I23" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K23" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="L23" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="M23" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N23" s="4" t="s">
+      <c r="N23" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="O23" s="4" t="s">
+      <c r="O23" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="P23" s="4" t="s">
+      <c r="P23" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="Q23" s="4" t="s">
+      <c r="Q23" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="R23" s="4" t="s">
+      <c r="R23" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="S23" s="27" t="s">
+      <c r="S23" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="T23" s="27" t="s">
+      <c r="T23" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="U23" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="V23" s="26"/>
+      <c r="U23" s="11" t="s">
+        <v>168</v>
+      </c>
       <c r="AA23" t="s">
         <v>54</v>
       </c>
@@ -3993,13 +4156,13 @@
       <c r="C24" s="1">
         <v>31</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="7">
         <v>1</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="7">
         <v>0.56732407424029996</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="7">
         <v>19.168641979741</v>
       </c>
       <c r="G24" s="1">
@@ -4019,10 +4182,10 @@
         <v>1824.8068659992102</v>
       </c>
       <c r="K24">
-        <f>J24/G24</f>
+        <f t="shared" ref="K24:K35" si="12">J24/G24</f>
         <v>0.17626603332422744</v>
       </c>
-      <c r="L24" s="25">
+      <c r="L24" s="24">
         <v>0.99366137766730001</v>
       </c>
       <c r="M24">
@@ -4038,11 +4201,11 @@
         <v>0.46795797207081591</v>
       </c>
       <c r="P24">
-        <f>C24*24</f>
+        <f t="shared" ref="P24:P35" si="13">C24*24</f>
         <v>744</v>
       </c>
       <c r="Q24">
-        <f>(O24/0.05)*C24*24</f>
+        <f t="shared" ref="Q24:Q35" si="14">(O24/0.05)*C24*24</f>
         <v>6963.2146244137402</v>
       </c>
       <c r="R24">
@@ -4050,7 +4213,7 @@
         <v>744</v>
       </c>
       <c r="S24">
-        <f>IF(Wärmequellen!$C$2=1,1,1-((10-D24)/22))</f>
+        <f>IF(Bilanzierung!$C$2=1,1,1-((10-D24)/22))</f>
         <v>0.59090909090909083</v>
       </c>
       <c r="T24">
@@ -4065,7 +4228,7 @@
         <v>55</v>
       </c>
       <c r="AB24">
-        <f>G24*N24*R24/1000</f>
+        <f t="shared" ref="AB24:AB35" si="15">G24*N24*R24/1000</f>
         <v>6353.2632040416711</v>
       </c>
     </row>
@@ -4076,13 +4239,13 @@
       <c r="C25" s="1">
         <v>28</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="7">
         <v>1.9</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="7">
         <v>0.54121604949352997</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="7">
         <v>19.208641979741</v>
       </c>
       <c r="G25" s="1">
@@ -4094,7 +4257,7 @@
         <v>9227.7345415439668</v>
       </c>
       <c r="I25">
-        <f t="shared" ref="I25:I35" si="12">IF(H25&lt;0,0,H25)</f>
+        <f t="shared" ref="I25:I35" si="16">IF(H25&lt;0,0,H25)</f>
         <v>9227.7345415439668</v>
       </c>
       <c r="J25">
@@ -4102,53 +4265,53 @@
         <v>1819.9885584688273</v>
       </c>
       <c r="K25">
-        <f>J25/G25</f>
+        <f t="shared" si="12"/>
         <v>0.18404496395395392</v>
       </c>
-      <c r="L25" s="25">
+      <c r="L25" s="24">
         <v>0.99311685252322002</v>
       </c>
       <c r="M25">
-        <f t="shared" ref="M25:M35" si="13">1-L25*K25</f>
+        <f t="shared" ref="M25:M35" si="17">1-L25*K25</f>
         <v>0.81722184467529979</v>
       </c>
       <c r="N25">
-        <f t="shared" ref="N25:N35" si="14">IF(M25&lt;=0,0,M25)</f>
+        <f t="shared" ref="N25:N35" si="18">IF(M25&lt;=0,0,M25)</f>
         <v>0.81722184467529979</v>
       </c>
       <c r="O25">
-        <f t="shared" ref="O25:O35" si="15">E25*N25</f>
+        <f t="shared" ref="O25:O35" si="19">E25*N25</f>
         <v>0.4422935783349809</v>
       </c>
       <c r="P25">
-        <f>C25*24</f>
+        <f t="shared" si="13"/>
         <v>672</v>
       </c>
       <c r="Q25">
-        <f>(O25/0.05)*C25*24</f>
+        <f t="shared" si="14"/>
         <v>5944.4256928221439</v>
       </c>
       <c r="R25">
-        <f t="shared" ref="R25:R35" si="16">IF(O25&gt;0.05,P25,Q25)</f>
+        <f t="shared" ref="R25:R35" si="20">IF(O25&gt;0.05,P25,Q25)</f>
         <v>672</v>
       </c>
       <c r="S25">
-        <f>IF(Wärmequellen!$C$2=1,1,1-((10-D25)/22))</f>
+        <f>IF(Bilanzierung!$C$2=1,1,1-((10-D25)/22))</f>
         <v>0.63181818181818183</v>
       </c>
       <c r="T25">
-        <f t="shared" ref="T25:T35" si="17">IF(24-S25*7&lt;17,17,24-S25*7)</f>
+        <f t="shared" ref="T25:T35" si="21">IF(24-S25*7&lt;17,17,24-S25*7)</f>
         <v>19.577272727272728</v>
       </c>
       <c r="U25">
-        <f t="shared" ref="U25:U35" si="18">R25*0.042*T25</f>
+        <f t="shared" ref="U25:U35" si="22">R25*0.042*T25</f>
         <v>552.54894545454545</v>
       </c>
       <c r="AA25" t="s">
         <v>56</v>
       </c>
       <c r="AB25">
-        <f>G25*N25*R25/1000</f>
+        <f t="shared" si="15"/>
         <v>5430.6768305859778</v>
       </c>
     </row>
@@ -4159,13 +4322,13 @@
       <c r="C26" s="1">
         <v>31</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="7">
         <v>4.7</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="7">
         <v>0.45721604949353001</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="7">
         <v>0</v>
       </c>
       <c r="G26" s="1">
@@ -4177,7 +4340,7 @@
         <v>2198.0499672886322</v>
       </c>
       <c r="I26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>2198.0499672886322</v>
       </c>
       <c r="J26">
@@ -4185,53 +4348,53 @@
         <v>2039.921565466685</v>
       </c>
       <c r="K26">
-        <f>J26/G26</f>
+        <f t="shared" si="12"/>
         <v>0.63505534376751283</v>
       </c>
-      <c r="L26" s="25">
+      <c r="L26" s="24">
         <v>0.88002952280601998</v>
       </c>
       <c r="M26">
+        <f t="shared" si="17"/>
+        <v>0.44113254886886266</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="18"/>
+        <v>0.44113254886886266</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="19"/>
+        <v>0.20169288129683297</v>
+      </c>
+      <c r="P26">
         <f t="shared" si="13"/>
-        <v>0.44113254886886266</v>
-      </c>
-      <c r="N26">
+        <v>744</v>
+      </c>
+      <c r="Q26">
         <f t="shared" si="14"/>
-        <v>0.44113254886886266</v>
-      </c>
-      <c r="O26">
-        <f t="shared" si="15"/>
-        <v>0.20169288129683297</v>
-      </c>
-      <c r="P26">
-        <f>C26*24</f>
+        <v>3001.1900736968746</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="20"/>
         <v>744</v>
       </c>
-      <c r="Q26">
-        <f>(O26/0.05)*C26*24</f>
-        <v>3001.1900736968746</v>
-      </c>
-      <c r="R26">
-        <f t="shared" si="16"/>
-        <v>744</v>
-      </c>
       <c r="S26">
-        <f>IF(Wärmequellen!$C$2=1,1,1-((10-D26)/22))</f>
+        <f>IF(Bilanzierung!$C$2=1,1,1-((10-D26)/22))</f>
         <v>0.75909090909090904</v>
       </c>
       <c r="T26">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>18.686363636363637</v>
       </c>
       <c r="U26">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>583.91149090909096</v>
       </c>
       <c r="AA26" t="s">
         <v>57</v>
       </c>
       <c r="AB26">
-        <f>G26*N26*R26/1000</f>
+        <f t="shared" si="15"/>
         <v>1054.2507854201413</v>
       </c>
     </row>
@@ -4242,13 +4405,13 @@
       <c r="C27" s="1">
         <v>30</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="7">
         <v>9.1999999999999993</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="7">
         <v>0.32310802474676997</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="7">
         <v>19.525401237337999</v>
       </c>
       <c r="G27" s="1">
@@ -4260,7 +4423,7 @@
         <v>4514.8736737870267</v>
       </c>
       <c r="I27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>4514.8736737870267</v>
       </c>
       <c r="J27">
@@ -4268,53 +4431,53 @@
         <v>2983.5729970125681</v>
       </c>
       <c r="K27">
-        <f>J27/G27</f>
+        <f t="shared" si="12"/>
         <v>0.50029840618168553</v>
       </c>
-      <c r="L27" s="25">
+      <c r="L27" s="24">
         <v>0.92689854189822996</v>
       </c>
       <c r="M27">
+        <f t="shared" si="17"/>
+        <v>0.5362741367961873</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="18"/>
+        <v>0.5362741367961873</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="19"/>
+        <v>0.1732744770629952</v>
+      </c>
+      <c r="P27">
         <f t="shared" si="13"/>
-        <v>0.5362741367961873</v>
-      </c>
-      <c r="N27">
+        <v>720</v>
+      </c>
+      <c r="Q27">
         <f t="shared" si="14"/>
-        <v>0.5362741367961873</v>
-      </c>
-      <c r="O27">
-        <f t="shared" si="15"/>
-        <v>0.1732744770629952</v>
-      </c>
-      <c r="P27">
-        <f>C27*24</f>
+        <v>2495.1524697071309</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="20"/>
         <v>720</v>
       </c>
-      <c r="Q27">
-        <f>(O27/0.05)*C27*24</f>
-        <v>2495.1524697071309</v>
-      </c>
-      <c r="R27">
-        <f t="shared" si="16"/>
-        <v>720</v>
-      </c>
       <c r="S27">
-        <f>IF(Wärmequellen!$C$2=1,1,1-((10-D27)/22))</f>
+        <f>IF(Bilanzierung!$C$2=1,1,1-((10-D27)/22))</f>
         <v>0.96363636363636362</v>
       </c>
       <c r="T27">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>17.254545454545454</v>
       </c>
       <c r="U27">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>521.77745454545459</v>
       </c>
       <c r="AA27" t="s">
         <v>58</v>
       </c>
       <c r="AB27">
-        <f>G27*N27*R27/1000</f>
+        <f t="shared" si="15"/>
         <v>2302.6445215805848</v>
       </c>
     </row>
@@ -4325,13 +4488,13 @@
       <c r="C28" s="1">
         <v>31</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="7">
         <v>14.1</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="7">
         <v>0.17610802474677001</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="7">
         <v>19.742160494935</v>
       </c>
       <c r="G28" s="1">
@@ -4343,7 +4506,7 @@
         <v>1763.6812418022057</v>
       </c>
       <c r="I28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1763.6812418022057</v>
       </c>
       <c r="J28">
@@ -4351,53 +4514,53 @@
         <v>2960.3998806143359</v>
       </c>
       <c r="K28">
-        <f>J28/G28</f>
+        <f t="shared" si="12"/>
         <v>0.90455622631620047</v>
       </c>
-      <c r="L28" s="25">
+      <c r="L28" s="24">
         <v>0.77826863399984003</v>
       </c>
       <c r="M28">
+        <f t="shared" si="17"/>
+        <v>0.29601226136884051</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="18"/>
+        <v>0.29601226136884051</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="19"/>
+        <v>5.2130134650491114E-2</v>
+      </c>
+      <c r="P28">
         <f t="shared" si="13"/>
-        <v>0.29601226136884051</v>
-      </c>
-      <c r="N28">
+        <v>744</v>
+      </c>
+      <c r="Q28">
         <f t="shared" si="14"/>
-        <v>0.29601226136884051</v>
-      </c>
-      <c r="O28">
-        <f t="shared" si="15"/>
-        <v>5.2130134650491114E-2</v>
-      </c>
-      <c r="P28">
-        <f>C28*24</f>
+        <v>775.69640359930781</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="20"/>
         <v>744</v>
       </c>
-      <c r="Q28">
-        <f>(O28/0.05)*C28*24</f>
-        <v>775.69640359930781</v>
-      </c>
-      <c r="R28">
-        <f t="shared" si="16"/>
-        <v>744</v>
-      </c>
       <c r="S28">
-        <f>IF(Wärmequellen!$C$2=1,1,1-((10-D28)/22))</f>
+        <f>IF(Bilanzierung!$C$2=1,1,1-((10-D28)/22))</f>
         <v>1.1863636363636363</v>
       </c>
       <c r="T28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>17</v>
       </c>
       <c r="U28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>531.21600000000001</v>
       </c>
       <c r="AA28" t="s">
         <v>59</v>
       </c>
       <c r="AB28">
-        <f>G28*N28*R28/1000</f>
+        <f t="shared" si="15"/>
         <v>720.77123617665859</v>
       </c>
     </row>
@@ -4408,13 +4571,13 @@
       <c r="C29" s="1">
         <v>30</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="7">
         <v>16.7</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="7">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="7">
         <v>19.852160494934999</v>
       </c>
       <c r="G29" s="1">
@@ -4426,7 +4589,7 @@
         <v>293.47716455620798</v>
       </c>
       <c r="I29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>293.47716455620798</v>
       </c>
       <c r="J29">
@@ -4434,53 +4597,53 @@
         <v>3048.6532362009584</v>
       </c>
       <c r="K29">
-        <f>J29/G29</f>
+        <f t="shared" si="12"/>
         <v>1.6513333718442131</v>
       </c>
-      <c r="L29" s="25">
+      <c r="L29" s="24">
         <v>0.54016665703894995</v>
       </c>
       <c r="M29">
+        <f t="shared" si="17"/>
+        <v>0.10800477287405408</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="18"/>
+        <v>0.10800477287405408</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="19"/>
+        <v>1.0692472514531355E-2</v>
+      </c>
+      <c r="P29">
         <f t="shared" si="13"/>
-        <v>0.10800477287405408</v>
-      </c>
-      <c r="N29">
+        <v>720</v>
+      </c>
+      <c r="Q29">
         <f t="shared" si="14"/>
-        <v>0.10800477287405408</v>
-      </c>
-      <c r="O29">
-        <f t="shared" si="15"/>
-        <v>1.0692472514531355E-2</v>
-      </c>
-      <c r="P29">
-        <f>C29*24</f>
-        <v>720</v>
-      </c>
-      <c r="Q29">
-        <f>(O29/0.05)*C29*24</f>
         <v>153.9716042092515</v>
       </c>
       <c r="R29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>153.9716042092515</v>
       </c>
       <c r="S29">
-        <f>IF(Wärmequellen!$C$2=1,1,1-((10-D29)/22))</f>
+        <f>IF(Bilanzierung!$C$2=1,1,1-((10-D29)/22))</f>
         <v>1.3045454545454545</v>
       </c>
       <c r="T29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>17</v>
       </c>
       <c r="U29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>109.93572540540558</v>
       </c>
       <c r="AA29" t="s">
         <v>60</v>
       </c>
       <c r="AB29">
-        <f>G29*N29*R29/1000</f>
+        <f t="shared" si="15"/>
         <v>30.701306266488476</v>
       </c>
     </row>
@@ -4491,13 +4654,13 @@
       <c r="C30" s="1">
         <v>31</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="7">
         <v>19</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="7">
         <v>0.03</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="7">
         <v>19.96</v>
       </c>
       <c r="G30" s="1">
@@ -4509,7 +4672,7 @@
         <v>-901.40430870463786</v>
       </c>
       <c r="I30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J30">
@@ -4517,53 +4680,53 @@
         <v>2836.6821047157532</v>
       </c>
       <c r="K30">
-        <f>J30/G30</f>
+        <f t="shared" si="12"/>
         <v>5.0533975106897957</v>
       </c>
-      <c r="L30" s="25">
+      <c r="L30" s="24">
         <v>0.19618448463655</v>
       </c>
       <c r="M30">
+        <f t="shared" si="17"/>
+        <v>8.6018137016977692E-3</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="18"/>
+        <v>8.6018137016977692E-3</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="19"/>
+        <v>2.5805441105093306E-4</v>
+      </c>
+      <c r="P30">
         <f t="shared" si="13"/>
-        <v>8.6018137016977692E-3</v>
-      </c>
-      <c r="N30">
+        <v>744</v>
+      </c>
+      <c r="Q30">
         <f t="shared" si="14"/>
-        <v>8.6018137016977692E-3</v>
-      </c>
-      <c r="O30">
-        <f t="shared" si="15"/>
-        <v>2.5805441105093306E-4</v>
-      </c>
-      <c r="P30">
-        <f>C30*24</f>
-        <v>744</v>
-      </c>
-      <c r="Q30">
-        <f>(O30/0.05)*C30*24</f>
         <v>3.8398496364378838</v>
       </c>
       <c r="R30">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>3.8398496364378838</v>
       </c>
       <c r="S30">
-        <f>IF(Wärmequellen!$C$2=1,1,1-((10-D30)/22))</f>
+        <f>IF(Bilanzierung!$C$2=1,1,1-((10-D30)/22))</f>
         <v>1.4090909090909092</v>
       </c>
       <c r="T30">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>17</v>
       </c>
       <c r="U30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>2.7416526404166492</v>
       </c>
       <c r="AA30" t="s">
         <v>61</v>
       </c>
       <c r="AB30">
-        <f>G30*N30*R30/1000</f>
+        <f t="shared" si="15"/>
         <v>1.8540927576451427E-2</v>
       </c>
     </row>
@@ -4574,13 +4737,13 @@
       <c r="C31" s="1">
         <v>31</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="7">
         <v>18.600000000000001</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="7">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="7">
         <v>19.940000000000001</v>
       </c>
       <c r="G31" s="1">
@@ -4592,7 +4755,7 @@
         <v>-567.44403772312535</v>
       </c>
       <c r="I31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J31">
@@ -4600,53 +4763,53 @@
         <v>2616.8512434657532</v>
       </c>
       <c r="K31">
-        <f>J31/G31</f>
+        <f t="shared" si="12"/>
         <v>3.3319283360319494</v>
       </c>
-      <c r="L31" s="25">
+      <c r="L31" s="24">
         <v>0.29344573311743999</v>
       </c>
       <c r="M31">
+        <f t="shared" si="17"/>
+        <v>2.22598467383327E-2</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="18"/>
+        <v>2.22598467383327E-2</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="19"/>
+        <v>9.3491356300997349E-4</v>
+      </c>
+      <c r="P31">
         <f t="shared" si="13"/>
-        <v>2.22598467383327E-2</v>
-      </c>
-      <c r="N31">
+        <v>744</v>
+      </c>
+      <c r="Q31">
         <f t="shared" si="14"/>
-        <v>2.22598467383327E-2</v>
-      </c>
-      <c r="O31">
-        <f t="shared" si="15"/>
-        <v>9.3491356300997349E-4</v>
-      </c>
-      <c r="P31">
-        <f>C31*24</f>
-        <v>744</v>
-      </c>
-      <c r="Q31">
-        <f>(O31/0.05)*C31*24</f>
         <v>13.911513817588403</v>
       </c>
       <c r="R31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>13.911513817588403</v>
       </c>
       <c r="S31">
-        <f>IF(Wärmequellen!$C$2=1,1,1-((10-D31)/22))</f>
+        <f>IF(Bilanzierung!$C$2=1,1,1-((10-D31)/22))</f>
         <v>1.3909090909090911</v>
       </c>
       <c r="T31">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>17</v>
       </c>
       <c r="U31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>9.9328208657581207</v>
       </c>
       <c r="AA31" t="s">
         <v>62</v>
       </c>
       <c r="AB31">
-        <f>G31*N31*R31/1000</f>
+        <f t="shared" si="15"/>
         <v>0.24320916963573855</v>
       </c>
     </row>
@@ -4657,13 +4820,13 @@
       <c r="C32" s="1">
         <v>30</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="7">
         <v>14.3</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="7">
         <v>0.17010802474677</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="7">
         <v>19.752160494935001</v>
       </c>
       <c r="G32" s="1">
@@ -4675,7 +4838,7 @@
         <v>2012.0949394546869</v>
       </c>
       <c r="I32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>2012.0949394546869</v>
       </c>
       <c r="J32">
@@ -4683,53 +4846,53 @@
         <v>2274.8838445947831</v>
       </c>
       <c r="K32">
-        <f>J32/G32</f>
+        <f t="shared" si="12"/>
         <v>0.7193859677129083</v>
       </c>
-      <c r="L32" s="25">
+      <c r="L32" s="24">
         <v>0.84863333226908999</v>
       </c>
       <c r="M32">
+        <f t="shared" si="17"/>
+        <v>0.38950508903217063</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="18"/>
+        <v>0.38950508903217063</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="19"/>
+        <v>6.6257941324077335E-2</v>
+      </c>
+      <c r="P32">
         <f t="shared" si="13"/>
-        <v>0.38950508903217063</v>
-      </c>
-      <c r="N32">
+        <v>720</v>
+      </c>
+      <c r="Q32">
         <f t="shared" si="14"/>
-        <v>0.38950508903217063</v>
-      </c>
-      <c r="O32">
-        <f t="shared" si="15"/>
-        <v>6.6257941324077335E-2</v>
-      </c>
-      <c r="P32">
-        <f>C32*24</f>
+        <v>954.11435506671341</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="20"/>
         <v>720</v>
       </c>
-      <c r="Q32">
-        <f>(O32/0.05)*C32*24</f>
-        <v>954.11435506671341</v>
-      </c>
-      <c r="R32">
-        <f t="shared" si="16"/>
-        <v>720</v>
-      </c>
       <c r="S32">
-        <f>IF(Wärmequellen!$C$2=1,1,1-((10-D32)/22))</f>
+        <f>IF(Bilanzierung!$C$2=1,1,1-((10-D32)/22))</f>
         <v>1.1954545454545455</v>
       </c>
       <c r="T32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>17</v>
       </c>
       <c r="U32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>514.08000000000004</v>
       </c>
       <c r="AA32" t="s">
         <v>63</v>
       </c>
       <c r="AB32">
-        <f>G32*N32*R32/1000</f>
+        <f t="shared" si="15"/>
         <v>886.83514750158997</v>
       </c>
     </row>
@@ -4740,13 +4903,13 @@
       <c r="C33" s="1">
         <v>31</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="7">
         <v>9.5</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="7">
         <v>0.31410802474677002</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="7">
         <v>19.535401237338</v>
       </c>
       <c r="G33" s="1">
@@ -4758,7 +4921,7 @@
         <v>4850.4791041953094</v>
       </c>
       <c r="I33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>4850.4791041953094</v>
       </c>
       <c r="J33">
@@ -4766,53 +4929,53 @@
         <v>1961.1296754658406</v>
       </c>
       <c r="K33">
-        <f>J33/G33</f>
+        <f t="shared" si="12"/>
         <v>0.3381658416229949</v>
       </c>
-      <c r="L33" s="25">
+      <c r="L33" s="24">
         <v>0.96960351484294005</v>
       </c>
       <c r="M33">
+        <f t="shared" si="17"/>
+        <v>0.67211321136252322</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="18"/>
+        <v>0.67211321136252322</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="19"/>
+        <v>0.21111615322729052</v>
+      </c>
+      <c r="P33">
         <f t="shared" si="13"/>
-        <v>0.67211321136252322</v>
-      </c>
-      <c r="N33">
+        <v>744</v>
+      </c>
+      <c r="Q33">
         <f t="shared" si="14"/>
-        <v>0.67211321136252322</v>
-      </c>
-      <c r="O33">
-        <f t="shared" si="15"/>
-        <v>0.21111615322729052</v>
-      </c>
-      <c r="P33">
-        <f>C33*24</f>
+        <v>3141.4083600220829</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="20"/>
         <v>744</v>
       </c>
-      <c r="Q33">
-        <f>(O33/0.05)*C33*24</f>
-        <v>3141.4083600220829</v>
-      </c>
-      <c r="R33">
-        <f t="shared" si="16"/>
-        <v>744</v>
-      </c>
       <c r="S33">
-        <f>IF(Wärmequellen!$C$2=1,1,1-((10-D33)/22))</f>
+        <f>IF(Bilanzierung!$C$2=1,1,1-((10-D33)/22))</f>
         <v>0.97727272727272729</v>
       </c>
       <c r="T33">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>17.15909090909091</v>
       </c>
       <c r="U33">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>536.18727272727278</v>
       </c>
       <c r="AA33" t="s">
         <v>64</v>
       </c>
       <c r="AB33">
-        <f>G33*N33*R33/1000</f>
+        <f t="shared" si="15"/>
         <v>2899.9595623428227</v>
       </c>
     </row>
@@ -4823,13 +4986,13 @@
       <c r="C34" s="1">
         <v>30</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="7">
         <v>0.47521604949353002</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F34" s="7">
         <v>19.306481484806</v>
       </c>
       <c r="G34" s="1">
@@ -4841,7 +5004,7 @@
         <v>8079.4411151744489</v>
       </c>
       <c r="I34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>8079.4411151744489</v>
       </c>
       <c r="J34">
@@ -4849,141 +5012,149 @@
         <v>1585.4541190044131</v>
       </c>
       <c r="K34">
-        <f>J34/G34</f>
+        <f t="shared" si="12"/>
         <v>0.1820242025955737</v>
       </c>
-      <c r="L34" s="25">
+      <c r="L34" s="24">
         <v>0.99325830581830998</v>
       </c>
       <c r="M34">
+        <f t="shared" si="17"/>
+        <v>0.81920294891199164</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="18"/>
+        <v>0.81920294891199164</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="19"/>
+        <v>0.38929838911540676</v>
+      </c>
+      <c r="P34">
         <f t="shared" si="13"/>
-        <v>0.81920294891199164</v>
-      </c>
-      <c r="N34">
+        <v>720</v>
+      </c>
+      <c r="Q34">
         <f t="shared" si="14"/>
-        <v>0.81920294891199164</v>
-      </c>
-      <c r="O34">
-        <f t="shared" si="15"/>
-        <v>0.38929838911540676</v>
-      </c>
-      <c r="P34">
-        <f>C34*24</f>
+        <v>5605.8968032618577</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="20"/>
         <v>720</v>
       </c>
-      <c r="Q34">
-        <f>(O34/0.05)*C34*24</f>
-        <v>5605.8968032618577</v>
-      </c>
-      <c r="R34">
-        <f t="shared" si="16"/>
-        <v>720</v>
-      </c>
       <c r="S34">
-        <f>IF(Wärmequellen!$C$2=1,1,1-((10-D34)/22))</f>
+        <f>IF(Bilanzierung!$C$2=1,1,1-((10-D34)/22))</f>
         <v>0.73181818181818181</v>
       </c>
       <c r="T34">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>18.877272727272725</v>
       </c>
       <c r="U34">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>570.84872727272727</v>
       </c>
       <c r="AA34" t="s">
         <v>65</v>
       </c>
       <c r="AB34">
-        <f>G34*N34*R34/1000</f>
+        <f t="shared" si="15"/>
         <v>5137.461080535214</v>
       </c>
     </row>
     <row r="35" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="26">
         <v>31</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="27">
         <v>0.9</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="27">
         <v>0.57032407424029996</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F35" s="27">
         <v>19.159722227208999</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G35" s="26">
         <f t="shared" si="11"/>
         <v>10404.338257532285</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="4">
         <f>G35-(F19+(0.5*R19)*Gebäude!I61)</f>
         <v>9829.1252726572857</v>
       </c>
-      <c r="I35">
-        <f t="shared" si="12"/>
+      <c r="I35" s="4">
+        <f t="shared" si="16"/>
         <v>9829.1252726572857</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="4">
         <f>AF19*Gebäude!I61</f>
         <v>1621.8764527572184</v>
       </c>
-      <c r="K35">
-        <f>J35/G35</f>
+      <c r="K35" s="4">
+        <f t="shared" si="12"/>
         <v>0.15588463318011128</v>
       </c>
-      <c r="L35" s="25">
+      <c r="L35" s="28">
         <v>0.99508807567738999</v>
       </c>
-      <c r="M35">
+      <c r="M35" s="4">
+        <f t="shared" si="17"/>
+        <v>0.8448810603411272</v>
+      </c>
+      <c r="N35" s="4">
+        <f t="shared" si="18"/>
+        <v>0.8448810603411272</v>
+      </c>
+      <c r="O35" s="4">
+        <f t="shared" si="19"/>
+        <v>0.48185600858221639</v>
+      </c>
+      <c r="P35" s="4">
         <f t="shared" si="13"/>
-        <v>0.8448810603411272</v>
-      </c>
-      <c r="N35">
+        <v>744</v>
+      </c>
+      <c r="Q35" s="4">
         <f t="shared" si="14"/>
-        <v>0.8448810603411272</v>
-      </c>
-      <c r="O35">
-        <f t="shared" si="15"/>
-        <v>0.48185600858221639</v>
-      </c>
-      <c r="P35">
-        <f>C35*24</f>
+        <v>7170.0174077033789</v>
+      </c>
+      <c r="R35" s="4">
+        <f t="shared" si="20"/>
         <v>744</v>
       </c>
-      <c r="Q35">
-        <f>(O35/0.05)*C35*24</f>
-        <v>7170.0174077033789</v>
-      </c>
-      <c r="R35">
-        <f t="shared" si="16"/>
-        <v>744</v>
-      </c>
-      <c r="S35">
-        <f>IF(Wärmequellen!$C$2=1,1,1-((10-D35)/22))</f>
+      <c r="S35" s="4">
+        <f>IF(Bilanzierung!$C$2=1,1,1-((10-D35)/22))</f>
         <v>0.58636363636363642</v>
       </c>
-      <c r="T35">
-        <f t="shared" si="17"/>
+      <c r="T35" s="4">
+        <f t="shared" si="21"/>
         <v>19.895454545454545</v>
       </c>
-      <c r="U35">
-        <f t="shared" si="18"/>
+      <c r="U35" s="4">
+        <f t="shared" si="22"/>
         <v>621.69316363636358</v>
       </c>
       <c r="AA35" s="4" t="s">
         <v>66</v>
       </c>
       <c r="AB35" s="4">
-        <f>G35*N35*R35/1000</f>
+        <f t="shared" si="15"/>
         <v>6540.0786843436945</v>
       </c>
     </row>
     <row r="36" spans="2:28" x14ac:dyDescent="0.2">
       <c r="K36" s="1"/>
+      <c r="R36">
+        <f>SUM(R24:R35)</f>
+        <v>6723.7229676632778</v>
+      </c>
+      <c r="U36" s="29">
+        <f>SUM(U24:U35)</f>
+        <v>5175.5721625479437</v>
+      </c>
       <c r="AA36" s="2" t="s">
         <v>127</v>
       </c>
@@ -4993,7 +5164,7 @@
       </c>
     </row>
     <row r="37" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="23" t="s">
         <v>77</v>
       </c>
       <c r="E37">
@@ -5002,19 +5173,17 @@
       </c>
     </row>
     <row r="38" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="S38" s="28" t="s">
-        <v>168</v>
-      </c>
+      <c r="S38" s="25"/>
     </row>
     <row r="39" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>78</v>
       </c>
-      <c r="K39" s="7"/>
+      <c r="K39" s="6"/>
     </row>
     <row r="40" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -5024,152 +5193,437 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9336C9-D30B-3E41-B0AD-8BF2B56C5439}">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E1DBB1D-9E50-6844-83C8-B5BC48EE082C}">
+  <dimension ref="B2:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1048576"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="5">
-        <v>31</v>
-      </c>
-      <c r="C1" s="5">
-        <v>0.56732407424029996</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="5">
-        <v>28</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0.54121604949352997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="5">
-        <v>31</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0.45721604949353001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="5">
-        <v>30</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0.32310802474676997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="5">
-        <v>31</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0.17610802474677001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="5">
-        <v>30</v>
-      </c>
-      <c r="C6" s="5">
-        <v>9.9000000000000005E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="5">
-        <v>31</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="5">
-        <v>31</v>
-      </c>
-      <c r="C8" s="5">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="H2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" t="str">
+        <f>Gebäude!B72</f>
+        <v>Ja</v>
+      </c>
+      <c r="E3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F3">
+        <f>Bilanzierung!AB36</f>
+        <v>31356.904108892053</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" t="str">
+        <f>Gebäude!B73</f>
+        <v>Nein</v>
+      </c>
+      <c r="E4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F4">
+        <f>Bilanzierung!R36</f>
+        <v>6723.7229676632778</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" t="str">
+        <f>Gebäude!B74</f>
+        <v>innerhalb</v>
+      </c>
+      <c r="E5" t="s">
+        <v>190</v>
+      </c>
+      <c r="F5">
+        <f>Gebäude!B64</f>
+        <v>15324.999551186025</v>
+      </c>
+      <c r="H5" t="s">
+        <v>194</v>
+      </c>
+      <c r="I5" t="s">
+        <v>197</v>
+      </c>
+      <c r="J5">
+        <v>1.099</v>
+      </c>
+      <c r="K5">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" t="str">
+        <f>Gebäude!B75</f>
+        <v>Ja</v>
+      </c>
+      <c r="E6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6">
+        <f>Gebäude!B16</f>
+        <v>324</v>
+      </c>
+      <c r="H6" t="s">
+        <v>194</v>
+      </c>
+      <c r="I6" t="s">
+        <v>198</v>
+      </c>
+      <c r="J6">
+        <v>1.07</v>
+      </c>
+      <c r="K6">
+        <v>1.0740000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" t="str">
+        <f>Gebäude!B76</f>
+        <v>flaechenheizung</v>
+      </c>
+      <c r="H7" t="s">
+        <v>194</v>
+      </c>
+      <c r="I7" t="s">
+        <v>199</v>
+      </c>
+      <c r="J7">
+        <v>1.0489999999999999</v>
+      </c>
+      <c r="K7">
+        <v>1.0549999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" t="str">
+        <f>Gebäude!B77</f>
+        <v>35/28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>194</v>
+      </c>
+      <c r="I8" t="s">
+        <v>180</v>
+      </c>
+      <c r="J8">
+        <v>1.0189999999999999</v>
+      </c>
+      <c r="K8">
+        <v>1.028</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" t="str">
+        <f>Gebäude!B78</f>
+        <v>35/28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>200</v>
+      </c>
+      <c r="I9" t="s">
+        <v>197</v>
+      </c>
+      <c r="J9">
+        <v>1.085</v>
+      </c>
+      <c r="K9">
+        <v>1.085</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" t="s">
+        <v>183</v>
+      </c>
+      <c r="H10" t="s">
+        <v>200</v>
+      </c>
+      <c r="I10" t="s">
+        <v>198</v>
+      </c>
+      <c r="J10">
+        <v>1.06</v>
+      </c>
+      <c r="K10">
+        <v>1.0629999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C11" t="str">
+        <f>Gebäude!B80</f>
+        <v>Nein</v>
+      </c>
+      <c r="H11" t="s">
+        <v>200</v>
+      </c>
+      <c r="I11" t="s">
+        <v>199</v>
+      </c>
+      <c r="J11">
+        <v>1.042</v>
+      </c>
+      <c r="K11">
+        <v>1.0469999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>202</v>
+      </c>
+      <c r="C12" t="str">
+        <f>Gebäude!B74</f>
+        <v>innerhalb</v>
+      </c>
+      <c r="H12" t="s">
+        <v>200</v>
+      </c>
+      <c r="I12" t="s">
+        <v>180</v>
+      </c>
+      <c r="J12">
+        <v>1.016</v>
+      </c>
+      <c r="K12">
+        <v>1.024</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13">
+        <f>Gebäude!B3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>210</v>
+      </c>
+      <c r="C14">
+        <f>Bilanzierung!U36</f>
+        <v>5175.5721625479437</v>
+      </c>
+      <c r="H14" t="s">
+        <v>201</v>
+      </c>
+      <c r="I14" t="str">
+        <f>IF(C13&lt;2,"EFH","MFH")</f>
+        <v>MFH</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>203</v>
+      </c>
+      <c r="I15" s="7">
+        <v>1.016</v>
+      </c>
+      <c r="J15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>179</v>
+      </c>
+      <c r="F16" cm="1">
+        <f t="array" ref="F16">_xlfn.SWITCH(C9,"90/70",1.042,"70/55",0.021,"55/45",0.015,"35/28",0.012)</f>
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E17" t="s">
+        <v>184</v>
+      </c>
+      <c r="F17" cm="1">
+        <f t="array" ref="F17">_xlfn.SWITCH(C10,"fussbodenheizung",0.021,"wandheizung",0.045,"deckenheizung",0.063)</f>
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>185</v>
+      </c>
+      <c r="F18">
+        <f>IF(C11="Ja",0.015,0.042)</f>
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="5">
-        <v>30</v>
-      </c>
-      <c r="C9" s="5">
-        <v>0.17010802474677</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="5">
-        <v>31</v>
-      </c>
-      <c r="C10" s="5">
-        <v>0.31410802474677002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="5">
-        <v>30</v>
-      </c>
-      <c r="C11" s="5">
-        <v>0.47521604949353002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="5">
-        <v>31</v>
-      </c>
-      <c r="C12" s="5">
-        <v>0.57032407424029996</v>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>174</v>
+      </c>
+      <c r="C19">
+        <f>IF(C7="elektroheizungsflaechen",1.066+0.018,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C20">
+        <f>IF(C7="heizkoerper",1.042+F16+0.009+0.03+0.036,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>176</v>
+      </c>
+      <c r="C21">
+        <f>IF(C7="flaechenheizung",1.042+F17+F18-0.03+0.036,0)</f>
+        <v>1.111</v>
+      </c>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>187</v>
+      </c>
+      <c r="C23" cm="1">
+        <f t="array" ref="C23">_xlfn.SWITCH(C7,"elektroheizungsflaechen",C19,"heizkoerper",C20,"flaechenheizung",C21)</f>
+        <v>1.111</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>188</v>
+      </c>
+      <c r="C24">
+        <f>(F3/(F4*F5))*1000</f>
+        <v>0.30431467521015609</v>
+      </c>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>191</v>
+      </c>
+      <c r="C25">
+        <f>(F5/F6)*C23</f>
+        <v>52.549612658542202</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>204</v>
+      </c>
+      <c r="C26">
+        <f>C24*C23*1.06</f>
+        <v>0.35837922040799247</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>206</v>
+      </c>
+      <c r="C27" s="7">
+        <v>1.0023351688163</v>
+      </c>
+      <c r="D27" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>203</v>
+      </c>
+      <c r="C28">
+        <f>I15</f>
+        <v>1.016</v>
+      </c>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29">
+        <f>C28*C27</f>
+        <v>1.0183725315173608</v>
+      </c>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30">
+        <f>1+(C29-1)*(50/C25)</f>
+        <v>1.0174811293441326</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>209</v>
+      </c>
+      <c r="C31">
+        <f>1+(C30-1)*(8760/C14)</f>
+        <v>1.0295879737051552</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Trinkwarmwasser aufgeräumt & Übergabe sowie Verteilung eingebaut
</commit_message>
<xml_diff>
--- a/din18599/Testberechnungen.xlsx
+++ b/din18599/Testberechnungen.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wagesve/Dev/Sites/enon/din18599/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA936236-F589-8642-AD46-8CE1E7E89AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BA811A-615E-8B4D-B221-646F5326B8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="3" xr2:uid="{7CF02650-DC02-AA49-AC3A-4487EF2FF614}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="4" xr2:uid="{7CF02650-DC02-AA49-AC3A-4487EF2FF614}"/>
   </bookViews>
   <sheets>
     <sheet name="Gebäude" sheetId="1" r:id="rId1"/>
     <sheet name="Dach" sheetId="2" r:id="rId2"/>
     <sheet name="Bilanzierung" sheetId="3" r:id="rId3"/>
     <sheet name="Heizung" sheetId="5" r:id="rId4"/>
+    <sheet name="Trinkwarmwasser" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="253">
   <si>
     <t>Haus Rechteckig</t>
   </si>
@@ -435,9 +436,6 @@
     <t>Ausrichtung</t>
   </si>
   <si>
-    <t>//Nord, Ost, Süd, West</t>
-  </si>
-  <si>
     <t>Fensterflächen nach Ausrichtung</t>
   </si>
   <si>
@@ -805,6 +803,24 @@
   </si>
   <si>
     <t>ehs</t>
+  </si>
+  <si>
+    <t>Standort Heizung</t>
+  </si>
+  <si>
+    <t>// Fixer Wert</t>
+  </si>
+  <si>
+    <t>Werte aus der Bilanzierung</t>
+  </si>
+  <si>
+    <t>Berechnete Werte</t>
+  </si>
+  <si>
+    <t>ewd</t>
+  </si>
+  <si>
+    <t>ewd0</t>
   </si>
 </sst>
 </file>
@@ -1068,7 +1084,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1385,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D0A30B-5A9B-F949-B5FE-8B73CA8912C0}">
   <dimension ref="A1:P88"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1410,7 +1426,7 @@
       <c r="B1" t="s">
         <v>48</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="3">
         <v>1990</v>
       </c>
     </row>
@@ -1552,9 +1568,6 @@
       </c>
       <c r="B7" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="C7" t="s">
-        <v>124</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>29</v>
@@ -1647,7 +1660,7 @@
         <v>44</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -1861,8 +1874,11 @@
       <c r="A19" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="28">
         <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>248</v>
       </c>
       <c r="G19" t="s">
         <v>28</v>
@@ -2292,7 +2308,7 @@
       </c>
       <c r="C48" s="6"/>
       <c r="G48" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -2306,10 +2322,10 @@
         <v>54</v>
       </c>
       <c r="H49" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I49" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -2535,54 +2551,54 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B69" s="7">
         <v>8.5</v>
       </c>
       <c r="C69" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>226</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>227</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B73" s="3"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B74" s="3"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C75" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>26</v>
@@ -2590,18 +2606,18 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>135</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="C77" t="s">
         <v>137</v>
-      </c>
-      <c r="C77" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>26</v>
@@ -2609,45 +2625,45 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>167</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C79" t="s">
         <v>168</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C79" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>179</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C82" t="s">
         <v>180</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C82" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>93</v>
@@ -2655,13 +2671,13 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B84" s="3"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B86">
         <f>IF(B77="innerhalb",IF(B78="Ja",1.554,0.647),IF(B78="Ja",0.815,0.335))</f>
@@ -2670,7 +2686,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B87">
         <f>IF(B78="Ja",1.321,0.451)</f>
@@ -2679,7 +2695,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B88" s="2">
         <f>IF(B75="Ja",IF(B76="Ja",B86,B87),0.193)</f>
@@ -2688,6 +2704,20 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B72:B74" xr:uid="{EDB12EEA-2178-8A41-89B4-DA86F44950E3}">
+      <formula1>"gasheizung,waermepumpe,biomassekessel"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B77" xr:uid="{3111FD3F-8FDF-BA45-98A0-84A9BF69D4A3}">
+      <formula1>"innerhalb,ausserhalb"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75 B76 B78 B83 B48 B49 B21 B22 B17" xr:uid="{3A890D37-40C6-5B45-88D5-3759B5891EA8}">
+      <formula1>"Ja,Nein"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{4D09400F-15BB-CC44-8D01-11722A6F7887}">
+      <formula1>"Nord,Ost,Süd,West"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -2858,8 +2888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A340B5-F068-DF4D-BA05-F7AD24B208A4}">
   <dimension ref="B2:AF40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2892,13 +2922,13 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F2" s="7">
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="G2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="2:32" x14ac:dyDescent="0.2">
@@ -2975,14 +3005,14 @@
         <v>11.9625</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U4">
         <f>Gebäude!B69</f>
         <v>8.5</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Y4">
         <f>Gebäude!B88</f>
@@ -3011,13 +3041,13 @@
       <c r="Q6" s="17"/>
       <c r="R6" s="18"/>
       <c r="T6" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AE6" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="AE6" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="7" spans="2:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3040,7 +3070,7 @@
         <v>54</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J7" s="10" t="s">
         <v>118</v>
@@ -3067,25 +3097,25 @@
         <v>121</v>
       </c>
       <c r="R7" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="T7" s="11" t="s">
         <v>54</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="V7" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="W7" s="11" t="s">
         <v>134</v>
-      </c>
-      <c r="W7" s="11" t="s">
-        <v>135</v>
       </c>
       <c r="AA7" s="2" t="s">
         <v>54</v>
       </c>
       <c r="AB7" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="2:32" x14ac:dyDescent="0.2">
@@ -4158,14 +4188,14 @@
     </row>
     <row r="20" spans="2:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F20" s="2">
         <f>SUM(F8:F19)</f>
         <v>5321.6999999999989</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N20">
         <f>SUM(N8:N19)</f>
@@ -4188,7 +4218,7 @@
         <v>11226.772665108001</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="U20" s="2"/>
       <c r="V20" s="2">
@@ -4200,7 +4230,7 @@
         <v>2139.8579999999997</v>
       </c>
       <c r="AA20" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AB20" s="2"/>
       <c r="AC20" s="2">
@@ -4208,7 +4238,7 @@
         <v>1779.2697025209013</v>
       </c>
       <c r="AE20" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AF20" s="2">
         <f>SUM(AF8:AF19)</f>
@@ -4220,7 +4250,7 @@
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
       <c r="AA22" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AB22" s="4"/>
     </row>
@@ -4232,7 +4262,7 @@
         <v>67</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>79</v>
@@ -4244,52 +4274,52 @@
         <v>107</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I23" s="11" t="s">
         <v>108</v>
       </c>
       <c r="J23" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="K23" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="K23" s="11" t="s">
+      <c r="L23" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="L23" s="11" t="s">
+      <c r="M23" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="N23" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="M23" s="11" t="s">
+      <c r="O23" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="N23" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="O23" s="11" t="s">
+      <c r="P23" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="P23" s="11" t="s">
+      <c r="Q23" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="Q23" s="11" t="s">
+      <c r="R23" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="R23" s="11" t="s">
-        <v>161</v>
-      </c>
       <c r="S23" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="T23" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="U23" s="11" t="s">
         <v>166</v>
-      </c>
-      <c r="T23" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="U23" s="11" t="s">
-        <v>167</v>
       </c>
       <c r="AA23" t="s">
         <v>54</v>
       </c>
       <c r="AB23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="2:32" x14ac:dyDescent="0.2">
@@ -5299,7 +5329,7 @@
         <v>5172.1584301122384</v>
       </c>
       <c r="AA36" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AB36" s="2">
         <f>SUM(AB24:AB35)</f>
@@ -5339,8 +5369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E1DBB1D-9E50-6844-83C8-B5BC48EE082C}">
   <dimension ref="B2:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5354,22 +5384,22 @@
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C3" t="str">
         <f>Gebäude!B75</f>
         <v>Ja</v>
       </c>
       <c r="E3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F3" t="str">
         <f>Gebäude!B72</f>
@@ -5378,52 +5408,52 @@
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C4" t="str">
         <f>Gebäude!B76</f>
         <v>Ja</v>
       </c>
       <c r="E4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F4">
         <f>Gebäude!B73</f>
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="J4" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C5" t="str">
         <f>Gebäude!B77</f>
         <v>innerhalb</v>
       </c>
       <c r="E5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F5">
         <f>Gebäude!B74</f>
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J5">
         <v>1.099</v>
@@ -5434,24 +5464,24 @@
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C6" t="str">
         <f>Gebäude!B78</f>
         <v>Ja</v>
       </c>
       <c r="E6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F6">
         <f>Bilanzierung!AB36</f>
         <v>31163.496960842906</v>
       </c>
       <c r="H6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J6">
         <v>1.07</v>
@@ -5462,24 +5492,24 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" t="str">
         <f>Gebäude!B79</f>
         <v>flaechenheizung</v>
       </c>
       <c r="E7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F7">
         <f>Bilanzierung!R36</f>
         <v>6718.9418297981456</v>
       </c>
       <c r="H7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J7">
         <v>1.0489999999999999</v>
@@ -5490,24 +5520,24 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C8" t="str">
         <f>Gebäude!B80</f>
         <v>35/28</v>
       </c>
       <c r="E8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F8">
         <f>Gebäude!B64</f>
         <v>15324.999551186025</v>
       </c>
       <c r="H8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J8">
         <v>1.0189999999999999</v>
@@ -5518,7 +5548,7 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C9" t="str">
         <f>Gebäude!B81</f>
@@ -5532,10 +5562,10 @@
         <v>324</v>
       </c>
       <c r="H9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J9">
         <v>1.085</v>
@@ -5546,16 +5576,16 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J10">
         <v>1.06</v>
@@ -5566,17 +5596,17 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C11" t="str">
         <f>Gebäude!B83</f>
         <v>Nein</v>
       </c>
       <c r="H11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J11">
         <v>1.042</v>
@@ -5587,17 +5617,17 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C12" t="str">
         <f>Gebäude!B77</f>
         <v>innerhalb</v>
       </c>
       <c r="H12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J12">
         <v>1.016</v>
@@ -5617,14 +5647,14 @@
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C14">
         <f>Bilanzierung!U36</f>
         <v>5172.1584301122384</v>
       </c>
       <c r="H14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I14" t="str">
         <f>IF(C13&lt;2,"EFH","MFH")</f>
@@ -5633,18 +5663,18 @@
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I15" s="7">
         <v>1.016</v>
       </c>
       <c r="J15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="E16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F16" cm="1">
         <f t="array" ref="F16">_xlfn.SWITCH(C9,"90/70",1.042,"70/55",0.021,"55/45",0.015,"35/28",0.012)</f>
@@ -5653,10 +5683,10 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F17" cm="1">
         <f t="array" ref="F17">_xlfn.SWITCH(C10,"fussbodenheizung",0.021,"wandheizung",0.045,"deckenheizung",0.063)</f>
@@ -5665,7 +5695,7 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F18">
         <f>IF(C11="Ja",0.015,0.042)</f>
@@ -5674,7 +5704,7 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C19">
         <f>IF(C7="elektroheizungsflaechen",1.066+0.018,0)</f>
@@ -5683,7 +5713,7 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C20">
         <f>IF(C7="heizkoerper",1.042+F16+0.009+0.03+0.036,0)</f>
@@ -5693,7 +5723,7 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C21">
         <f>IF(C7="flaechenheizung",1.042+F17+F18-0.03+0.036,0)</f>
@@ -5703,7 +5733,7 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C23" cm="1">
         <f t="array" ref="C23">_xlfn.SWITCH(C7,"elektroheizungsflaechen",C19,"heizkoerper",C20,"flaechenheizung",C21)</f>
@@ -5712,7 +5742,7 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C24">
         <f>(F6/(F7*F8))*1000</f>
@@ -5722,7 +5752,7 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C25">
         <f>(F8/F9)*C23</f>
@@ -5731,7 +5761,7 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C26">
         <f>C24*C23*1.06</f>
@@ -5740,18 +5770,18 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C27" s="7">
         <v>1.0022568883755001</v>
       </c>
       <c r="D27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C28">
         <f>I15</f>
@@ -5761,7 +5791,7 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C29">
         <f>C28*C27</f>
@@ -5771,7 +5801,7 @@
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C30">
         <f>1+(C29-1)*(50/C25)</f>
@@ -5780,7 +5810,7 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C31">
         <f>1+(C30-1)*(8760/C14)</f>
@@ -5789,7 +5819,7 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C32">
         <f>Bilanzierung!V20</f>
@@ -5798,7 +5828,7 @@
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C33">
         <f>Bilanzierung!U36</f>
@@ -5807,12 +5837,12 @@
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C37" t="str">
         <f>Gebäude!B76</f>
@@ -5821,7 +5851,7 @@
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C38" t="str">
         <f>Gebäude!B75</f>
@@ -5838,8 +5868,8 @@
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="28" t="s">
-        <v>229</v>
+      <c r="B40" t="s">
+        <v>228</v>
       </c>
       <c r="C40" t="str">
         <f>IF(OR(F3="biomassekessel",F4="biomassekessel",F5="biomassekessel"),"Ja","Nein")</f>
@@ -5847,8 +5877,8 @@
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="28" t="s">
-        <v>232</v>
+      <c r="B41" t="s">
+        <v>231</v>
       </c>
       <c r="C41" t="str">
         <f>IF(OR(F3="waermepumpe",F4="waermepumpe",F5="waermepumpe"),"Ja","Nein")</f>
@@ -5857,18 +5887,18 @@
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C43" s="7">
         <v>1.0736222287534001</v>
       </c>
       <c r="D43" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C44">
         <f>C43*C33/5000</f>
@@ -5877,7 +5907,7 @@
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C45">
         <f>C26*C31</f>
@@ -5885,47 +5915,47 @@
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B47" s="28" t="s">
-        <v>215</v>
+      <c r="B47" t="s">
+        <v>214</v>
       </c>
       <c r="C47" s="7">
         <v>18436</v>
       </c>
       <c r="D47" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E47" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B48" s="28" t="s">
-        <v>216</v>
+      <c r="B48" t="s">
+        <v>215</v>
       </c>
       <c r="C48">
         <f>0.42*POWER(((C32*C39)/(365*0.036)),0.7)</f>
         <v>623.54499849662818</v>
       </c>
       <c r="D48" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E48" s="6"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C49">
         <f>IF(C39&gt;5000,C48/1000,C47/1000)</f>
         <v>18.436</v>
       </c>
       <c r="D49" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C51">
         <f>IF(AND(C3="Ja",C41="Nein"),1.5*C49,0)</f>
@@ -5934,7 +5964,7 @@
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C52">
         <f>IF(AND(C3="Ja",C41="Ja"),1.3*F8/1000,0)</f>
@@ -5943,7 +5973,7 @@
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C53">
         <f>IF(AND(C3="Nein",C41="Nein"),1.5*C49,0)</f>
@@ -5952,7 +5982,7 @@
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C54">
         <f>IF(AND(C3="Nein",C41="Ja"),F8/1000,0)</f>
@@ -5961,7 +5991,7 @@
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C55">
         <f>SUM(C51:C54)</f>
@@ -5970,7 +6000,7 @@
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C57">
         <f>IF(C40="Ja",50*C55,0)</f>
@@ -5979,7 +6009,7 @@
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C58">
         <f>IF(AND(C40="Nein",C41="Ja"),9.5*C55,0)</f>
@@ -5988,7 +6018,7 @@
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C59">
         <f>SUM(C57:C58)</f>
@@ -5997,7 +6027,7 @@
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C61">
         <f>IF(C59&gt;1500,1500,C59)</f>
@@ -6006,7 +6036,7 @@
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C62">
         <f>IF(C59&gt;1500,C59-C61,0)</f>
@@ -6015,18 +6045,18 @@
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C64" s="7">
         <v>49.604286779429003</v>
       </c>
       <c r="E64" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C65" s="7">
         <v>0</v>
@@ -6034,7 +6064,7 @@
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B66" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C66">
         <f>SUM(C64:C65)</f>
@@ -6043,7 +6073,7 @@
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B68" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C68">
         <f>1+C66/(F6*C23*C31)</f>
@@ -6056,4 +6086,86 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9A3F0F-1C91-984E-A382-DFE3170310F1}">
+  <dimension ref="B2:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" t="str">
+        <f>Gebäude!B75</f>
+        <v>Ja</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" t="str">
+        <f>Gebäude!B77</f>
+        <v>innerhalb</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7">
+        <f>Bilanzierung!V20</f>
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>252</v>
+      </c>
+      <c r="C10">
+        <f>IF(C3="Ja",IF(C4="innerhalb",2.252,2.29),1.193)</f>
+        <v>2.2519999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>251</v>
+      </c>
+      <c r="C11">
+        <f>1+(C10-1)*(12.5/C7)</f>
+        <v>1.011365286855483</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E12" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Speichern vor dem Wochenende
</commit_message>
<xml_diff>
--- a/din18599/Testberechnungen.xlsx
+++ b/din18599/Testberechnungen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wagesve/Dev/Sites/enon/din18599/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7EDF6B-DB4A-C349-AB47-4FB45A8E2CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5C3D2B-F06B-8041-B672-75FAE5D404B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="4" xr2:uid="{7CF02650-DC02-AA49-AC3A-4487EF2FF614}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" activeTab="4" xr2:uid="{7CF02650-DC02-AA49-AC3A-4487EF2FF614}"/>
   </bookViews>
   <sheets>
     <sheet name="Gebäude" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="257">
   <si>
     <t>Haus Rechteckig</t>
   </si>
@@ -824,6 +824,15 @@
   </si>
   <si>
     <t>Speicherung</t>
+  </si>
+  <si>
+    <t>fwb</t>
+  </si>
+  <si>
+    <t>// $fwb = ($qwb/12,5)*/((1+($ewd0-1))*(12,5/$qwb)/$ewd0)</t>
+  </si>
+  <si>
+    <t>Nutzwärmebedarf Trinnkwasser</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1065,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1087,7 +1096,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1404,7 +1412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D0A30B-5A9B-F949-B5FE-8B73CA8912C0}">
   <dimension ref="A1:P88"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
@@ -1877,7 +1885,7 @@
       <c r="A19" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="28">
+      <c r="B19">
         <v>50</v>
       </c>
       <c r="C19" t="s">
@@ -2891,8 +2899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A340B5-F068-DF4D-BA05-F7AD24B208A4}">
   <dimension ref="B2:AF40"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5372,7 +5380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E1DBB1D-9E50-6844-83C8-B5BC48EE082C}">
   <dimension ref="B2:K68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6093,10 +6101,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9A3F0F-1C91-984E-A382-DFE3170310F1}">
-  <dimension ref="B2:E13"/>
+  <dimension ref="B2:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6141,39 +6149,57 @@
         <v>1377</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>256</v>
+      </c>
+      <c r="C8">
+        <f>Bilanzierung!U4</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>251</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <f>IF(C3="Ja",IF(C4="innerhalb",2.252,2.29),1.193)</f>
         <v>2.2519999999999998</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>250</v>
       </c>
-      <c r="C11">
-        <f>1+(C10-1)*(12.5/C7)</f>
+      <c r="C12">
+        <f>1+(C11-1)*(12.5/C7)</f>
         <v>1.011365286855483</v>
       </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
         <v>253</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>254</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Komma aus Spalten entfernt
</commit_message>
<xml_diff>
--- a/din18599/Testberechnungen.xlsx
+++ b/din18599/Testberechnungen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wagesve/Dev/Sites/enon/din18599/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0BBD8C-F562-2D48-B405-F4C7906BD05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE7E739-0CD2-CB43-8574-0083A31D03BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-51200" yWindow="-9160" windowWidth="51200" windowHeight="28800" activeTab="4" xr2:uid="{7CF02650-DC02-AA49-AC3A-4487EF2FF614}"/>
   </bookViews>
@@ -6237,8 +6237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9A3F0F-1C91-984E-A382-DFE3170310F1}">
   <dimension ref="B2:M79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6753,8 +6753,8 @@
         <v>296</v>
       </c>
       <c r="C79">
-        <f>1+(C77/C9*C14*1)</f>
-        <v>1.1049866692210986</v>
+        <f>1+(C77/(C9*C14*1))</f>
+        <v>1.1026403374389782</v>
       </c>
     </row>
   </sheetData>

</xml_diff>